<commit_message>
route fixed, no looping :(, suggested speeds, authority fully functional
</commit_message>
<xml_diff>
--- a/modules/Green Line Info_.xlsx
+++ b/modules/Green Line Info_.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Desktop\School\1140\1140_iteration4\1140\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/52e6f4f7f86bcef2/Desktop/School/1140/1140/modules/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D4B131F-9DEC-48BC-972F-271BE62DE00D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="12" documentId="13_ncr:1_{8D4B131F-9DEC-48BC-972F-271BE62DE00D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B6296A60-270B-4979-9730-87888BC513B6}"/>
   <bookViews>
-    <workbookView xWindow="492" yWindow="912" windowWidth="17280" windowHeight="8964" xr2:uid="{74BABC91-B30C-4EA1-9E18-CB507E7797A1}"/>
+    <workbookView xWindow="220" yWindow="570" windowWidth="28800" windowHeight="15460" xr2:uid="{74BABC91-B30C-4EA1-9E18-CB507E7797A1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -116,9 +116,6 @@
     <t>W</t>
   </si>
   <si>
-    <t>Speed Limit (Km/Hr)</t>
-  </si>
-  <si>
     <t>Infrastructure</t>
   </si>
   <si>
@@ -183,6 +180,9 @@
   </si>
   <si>
     <t>Y</t>
+  </si>
+  <si>
+    <t>Speed Limit (m/s)</t>
   </si>
 </sst>
 </file>
@@ -265,6 +265,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -564,18 +568,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E4104CD2-E043-4597-AF7D-F6AD80AEEABB}">
-  <dimension ref="A1:E224"/>
+  <dimension ref="A1:F224"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A169" workbookViewId="0">
-      <selection activeCell="A174" sqref="A174:E174"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="5" max="5" width="37.5546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="37.54296875" style="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="46.8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" ht="46.5" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -586,15 +590,19 @@
         <v>2</v>
       </c>
       <c r="D1" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F1" t="e">
+        <f>D1*0.27777778</f>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B2" s="5">
         <v>151</v>
@@ -603,13 +611,17 @@
         <v>50</v>
       </c>
       <c r="D2" s="5">
-        <v>100</v>
+        <v>27.777777999999998</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+        <v>45</v>
+      </c>
+      <c r="F2">
+        <f t="shared" ref="F2:F65" si="0">D2*0.27777778</f>
+        <v>7.7160495061728387</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" s="3" t="s">
         <v>12</v>
       </c>
@@ -620,13 +632,17 @@
         <v>50</v>
       </c>
       <c r="D3" s="3">
-        <v>60</v>
+        <v>16.666666799999998</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+        <v>36</v>
+      </c>
+      <c r="F3">
+        <f t="shared" si="0"/>
+        <v>4.6296297037037029</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">
         <v>13</v>
       </c>
@@ -637,10 +653,14 @@
         <v>100</v>
       </c>
       <c r="D4" s="3">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+        <v>19.444444599999997</v>
+      </c>
+      <c r="F4">
+        <f t="shared" si="0"/>
+        <v>5.4012346543209864</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" s="3" t="s">
         <v>13</v>
       </c>
@@ -651,10 +671,14 @@
         <v>100</v>
       </c>
       <c r="D5" s="3">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+        <v>19.444444599999997</v>
+      </c>
+      <c r="F5">
+        <f t="shared" si="0"/>
+        <v>5.4012346543209864</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" s="3" t="s">
         <v>13</v>
       </c>
@@ -665,13 +689,17 @@
         <v>200</v>
       </c>
       <c r="D6" s="3">
-        <v>70</v>
+        <v>19.444444599999997</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+        <v>37</v>
+      </c>
+      <c r="F6">
+        <f t="shared" si="0"/>
+        <v>5.4012346543209864</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" s="3" t="s">
         <v>13</v>
       </c>
@@ -682,10 +710,14 @@
         <v>200</v>
       </c>
       <c r="D7" s="3">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+        <v>19.444444599999997</v>
+      </c>
+      <c r="F7">
+        <f t="shared" si="0"/>
+        <v>5.4012346543209864</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8" s="3" t="s">
         <v>13</v>
       </c>
@@ -696,10 +728,14 @@
         <v>100</v>
       </c>
       <c r="D8" s="3">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+        <v>19.444444599999997</v>
+      </c>
+      <c r="F8">
+        <f t="shared" si="0"/>
+        <v>5.4012346543209864</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A9" s="3" t="s">
         <v>13</v>
       </c>
@@ -710,10 +746,14 @@
         <v>100</v>
       </c>
       <c r="D9" s="3">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+        <v>19.444444599999997</v>
+      </c>
+      <c r="F9">
+        <f t="shared" si="0"/>
+        <v>5.4012346543209864</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A10" s="3" t="s">
         <v>14</v>
       </c>
@@ -724,10 +764,14 @@
         <v>100</v>
       </c>
       <c r="D10" s="3">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+        <v>16.666666799999998</v>
+      </c>
+      <c r="F10">
+        <f t="shared" si="0"/>
+        <v>4.6296297037037029</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A11" s="3" t="s">
         <v>14</v>
       </c>
@@ -738,10 +782,14 @@
         <v>100</v>
       </c>
       <c r="D11" s="3">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+        <v>16.666666799999998</v>
+      </c>
+      <c r="F11">
+        <f t="shared" si="0"/>
+        <v>4.6296297037037029</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A12" s="3" t="s">
         <v>14</v>
       </c>
@@ -752,10 +800,14 @@
         <v>100</v>
       </c>
       <c r="D12" s="3">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+        <v>16.666666799999998</v>
+      </c>
+      <c r="F12">
+        <f t="shared" si="0"/>
+        <v>4.6296297037037029</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A13" s="3" t="s">
         <v>14</v>
       </c>
@@ -766,10 +818,14 @@
         <v>100</v>
       </c>
       <c r="D13" s="3">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+        <v>16.666666799999998</v>
+      </c>
+      <c r="F13">
+        <f t="shared" si="0"/>
+        <v>4.6296297037037029</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A14" s="3" t="s">
         <v>14</v>
       </c>
@@ -780,13 +836,17 @@
         <v>100</v>
       </c>
       <c r="D14" s="3">
-        <v>60</v>
+        <v>16.666666799999998</v>
       </c>
       <c r="E14" s="5" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+        <v>38</v>
+      </c>
+      <c r="F14">
+        <f t="shared" si="0"/>
+        <v>4.6296297037037029</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A15" s="3" t="s">
         <v>15</v>
       </c>
@@ -797,10 +857,14 @@
         <v>100</v>
       </c>
       <c r="D15" s="3">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+        <v>16.666666799999998</v>
+      </c>
+      <c r="F15">
+        <f t="shared" si="0"/>
+        <v>4.6296297037037029</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A16" s="3" t="s">
         <v>15</v>
       </c>
@@ -811,10 +875,14 @@
         <v>100</v>
       </c>
       <c r="D16" s="3">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+        <v>16.666666799999998</v>
+      </c>
+      <c r="F16">
+        <f t="shared" si="0"/>
+        <v>4.6296297037037029</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A17" s="3" t="s">
         <v>15</v>
       </c>
@@ -825,13 +893,17 @@
         <v>100</v>
       </c>
       <c r="D17" s="3">
-        <v>60</v>
+        <v>16.666666799999998</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+        <v>29</v>
+      </c>
+      <c r="F17">
+        <f t="shared" si="0"/>
+        <v>4.6296297037037029</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A18" s="3" t="s">
         <v>16</v>
       </c>
@@ -842,13 +914,17 @@
         <v>300</v>
       </c>
       <c r="D18" s="3">
-        <v>70</v>
+        <v>19.444444599999997</v>
       </c>
       <c r="E18" s="5" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+        <v>39</v>
+      </c>
+      <c r="F18">
+        <f t="shared" si="0"/>
+        <v>5.4012346543209864</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A19" s="3" t="s">
         <v>16</v>
       </c>
@@ -859,10 +935,14 @@
         <v>300</v>
       </c>
       <c r="D19" s="3">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+        <v>19.444444599999997</v>
+      </c>
+      <c r="F19">
+        <f t="shared" si="0"/>
+        <v>5.4012346543209864</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A20" s="3" t="s">
         <v>16</v>
       </c>
@@ -873,10 +953,14 @@
         <v>300</v>
       </c>
       <c r="D20" s="3">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+        <v>19.444444599999997</v>
+      </c>
+      <c r="F20">
+        <f t="shared" si="0"/>
+        <v>5.4012346543209864</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A21" s="3" t="s">
         <v>16</v>
       </c>
@@ -887,10 +971,14 @@
         <v>300</v>
       </c>
       <c r="D21" s="3">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+        <v>19.444444599999997</v>
+      </c>
+      <c r="F21">
+        <f t="shared" si="0"/>
+        <v>5.4012346543209864</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A22" s="3" t="s">
         <v>16</v>
       </c>
@@ -901,10 +989,14 @@
         <v>300</v>
       </c>
       <c r="D22" s="3">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+        <v>19.444444599999997</v>
+      </c>
+      <c r="F22">
+        <f t="shared" si="0"/>
+        <v>5.4012346543209864</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A23" s="3" t="s">
         <v>16</v>
       </c>
@@ -915,10 +1007,14 @@
         <v>300</v>
       </c>
       <c r="D23" s="3">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+        <v>19.444444599999997</v>
+      </c>
+      <c r="F23">
+        <f t="shared" si="0"/>
+        <v>5.4012346543209864</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A24" s="3" t="s">
         <v>16</v>
       </c>
@@ -929,10 +1025,14 @@
         <v>300</v>
       </c>
       <c r="D24" s="3">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+        <v>19.444444599999997</v>
+      </c>
+      <c r="F24">
+        <f t="shared" si="0"/>
+        <v>5.4012346543209864</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A25" s="3" t="s">
         <v>16</v>
       </c>
@@ -943,10 +1043,14 @@
         <v>300</v>
       </c>
       <c r="D25" s="3">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+        <v>19.444444599999997</v>
+      </c>
+      <c r="F25">
+        <f t="shared" si="0"/>
+        <v>5.4012346543209864</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A26" s="3" t="s">
         <v>16</v>
       </c>
@@ -957,10 +1061,14 @@
         <v>300</v>
       </c>
       <c r="D26" s="3">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+        <v>19.444444599999997</v>
+      </c>
+      <c r="F26">
+        <f t="shared" si="0"/>
+        <v>5.4012346543209864</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A27" s="3" t="s">
         <v>17</v>
       </c>
@@ -971,13 +1079,17 @@
         <v>100</v>
       </c>
       <c r="D27" s="3">
-        <v>55</v>
+        <v>15.277777899999998</v>
       </c>
       <c r="E27" s="3" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+        <v>29</v>
+      </c>
+      <c r="F27">
+        <f t="shared" si="0"/>
+        <v>4.2438272283950615</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A28" s="3" t="s">
         <v>17</v>
       </c>
@@ -988,10 +1100,14 @@
         <v>86.6</v>
       </c>
       <c r="D28" s="3">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+        <v>15.277777899999998</v>
+      </c>
+      <c r="F28">
+        <f t="shared" si="0"/>
+        <v>4.2438272283950615</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A29" s="3" t="s">
         <v>17</v>
       </c>
@@ -1002,13 +1118,17 @@
         <v>100</v>
       </c>
       <c r="D29" s="3">
-        <v>55</v>
+        <v>15.277777899999998</v>
       </c>
       <c r="E29" s="5" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+        <v>40</v>
+      </c>
+      <c r="F29">
+        <f t="shared" si="0"/>
+        <v>4.2438272283950615</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A30" s="3" t="s">
         <v>18</v>
       </c>
@@ -1019,10 +1139,14 @@
         <v>75</v>
       </c>
       <c r="D30" s="3">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+        <v>15.277777899999998</v>
+      </c>
+      <c r="F30">
+        <f t="shared" si="0"/>
+        <v>4.2438272283950615</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A31" s="3" t="s">
         <v>18</v>
       </c>
@@ -1033,10 +1157,14 @@
         <v>75</v>
       </c>
       <c r="D31" s="3">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+        <v>15.277777899999998</v>
+      </c>
+      <c r="F31">
+        <f t="shared" si="0"/>
+        <v>4.2438272283950615</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A32" s="3" t="s">
         <v>18</v>
       </c>
@@ -1047,10 +1175,14 @@
         <v>75</v>
       </c>
       <c r="D32" s="3">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+        <v>15.277777899999998</v>
+      </c>
+      <c r="F32">
+        <f t="shared" si="0"/>
+        <v>4.2438272283950615</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A33" s="3" t="s">
         <v>18</v>
       </c>
@@ -1061,10 +1193,14 @@
         <v>75</v>
       </c>
       <c r="D33" s="3">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+        <v>15.277777899999998</v>
+      </c>
+      <c r="F33">
+        <f t="shared" si="0"/>
+        <v>4.2438272283950615</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A34" s="3" t="s">
         <v>18</v>
       </c>
@@ -1075,10 +1211,14 @@
         <v>75</v>
       </c>
       <c r="D34" s="3">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+        <v>15.277777899999998</v>
+      </c>
+      <c r="F34">
+        <f t="shared" si="0"/>
+        <v>4.2438272283950615</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A35" s="3" t="s">
         <v>18</v>
       </c>
@@ -1089,10 +1229,14 @@
         <v>75</v>
       </c>
       <c r="D35" s="3">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+        <v>15.277777899999998</v>
+      </c>
+      <c r="F35">
+        <f t="shared" si="0"/>
+        <v>4.2438272283950615</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A36" s="3" t="s">
         <v>18</v>
       </c>
@@ -1103,10 +1247,14 @@
         <v>75</v>
       </c>
       <c r="D36" s="3">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+        <v>15.277777899999998</v>
+      </c>
+      <c r="F36">
+        <f t="shared" si="0"/>
+        <v>4.2438272283950615</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A37" s="3" t="s">
         <v>18</v>
       </c>
@@ -1117,13 +1265,17 @@
         <v>75</v>
       </c>
       <c r="D37" s="3">
-        <v>55</v>
+        <v>15.277777899999998</v>
       </c>
       <c r="E37" s="5" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
+        <v>41</v>
+      </c>
+      <c r="F37">
+        <f t="shared" si="0"/>
+        <v>4.2438272283950615</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A38" s="3" t="s">
         <v>18</v>
       </c>
@@ -1134,10 +1286,14 @@
         <v>75</v>
       </c>
       <c r="D38" s="3">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
+        <v>15.277777899999998</v>
+      </c>
+      <c r="F38">
+        <f t="shared" si="0"/>
+        <v>4.2438272283950615</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A39" s="3" t="s">
         <v>19</v>
       </c>
@@ -1148,10 +1304,14 @@
         <v>75</v>
       </c>
       <c r="D39" s="3">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
+        <v>15.277777899999998</v>
+      </c>
+      <c r="F39">
+        <f t="shared" si="0"/>
+        <v>4.2438272283950615</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A40" s="3" t="s">
         <v>19</v>
       </c>
@@ -1162,10 +1322,14 @@
         <v>75</v>
       </c>
       <c r="D40" s="3">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
+        <v>15.277777899999998</v>
+      </c>
+      <c r="F40">
+        <f t="shared" si="0"/>
+        <v>4.2438272283950615</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A41" s="3" t="s">
         <v>19</v>
       </c>
@@ -1176,10 +1340,14 @@
         <v>75</v>
       </c>
       <c r="D41" s="3">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
+        <v>15.277777899999998</v>
+      </c>
+      <c r="F41">
+        <f t="shared" si="0"/>
+        <v>4.2438272283950615</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A42" s="3" t="s">
         <v>16</v>
       </c>
@@ -1190,10 +1358,14 @@
         <v>300</v>
       </c>
       <c r="D42" s="3">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
+        <v>19.444444599999997</v>
+      </c>
+      <c r="F42">
+        <f t="shared" si="0"/>
+        <v>5.4012346543209864</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A43" s="3" t="s">
         <v>16</v>
       </c>
@@ -1204,10 +1376,14 @@
         <v>300</v>
       </c>
       <c r="D43" s="3">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
+        <v>19.444444599999997</v>
+      </c>
+      <c r="F43">
+        <f t="shared" si="0"/>
+        <v>5.4012346543209864</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A44" s="3" t="s">
         <v>16</v>
       </c>
@@ -1218,10 +1394,14 @@
         <v>300</v>
       </c>
       <c r="D44" s="3">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
+        <v>19.444444599999997</v>
+      </c>
+      <c r="F44">
+        <f t="shared" si="0"/>
+        <v>5.4012346543209864</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A45" s="3" t="s">
         <v>16</v>
       </c>
@@ -1232,10 +1412,14 @@
         <v>300</v>
       </c>
       <c r="D45" s="3">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
+        <v>19.444444599999997</v>
+      </c>
+      <c r="F45">
+        <f t="shared" si="0"/>
+        <v>5.4012346543209864</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A46" s="3" t="s">
         <v>16</v>
       </c>
@@ -1246,10 +1430,14 @@
         <v>300</v>
       </c>
       <c r="D46" s="3">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
+        <v>19.444444599999997</v>
+      </c>
+      <c r="F46">
+        <f t="shared" si="0"/>
+        <v>5.4012346543209864</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A47" s="3" t="s">
         <v>16</v>
       </c>
@@ -1260,10 +1448,14 @@
         <v>300</v>
       </c>
       <c r="D47" s="3">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
+        <v>19.444444599999997</v>
+      </c>
+      <c r="F47">
+        <f t="shared" si="0"/>
+        <v>5.4012346543209864</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A48" s="3" t="s">
         <v>16</v>
       </c>
@@ -1274,10 +1466,14 @@
         <v>300</v>
       </c>
       <c r="D48" s="3">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
+        <v>19.444444599999997</v>
+      </c>
+      <c r="F48">
+        <f t="shared" si="0"/>
+        <v>5.4012346543209864</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A49" s="3" t="s">
         <v>16</v>
       </c>
@@ -1288,10 +1484,14 @@
         <v>300</v>
       </c>
       <c r="D49" s="3">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
+        <v>19.444444599999997</v>
+      </c>
+      <c r="F49">
+        <f t="shared" si="0"/>
+        <v>5.4012346543209864</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A50" s="3" t="s">
         <v>16</v>
       </c>
@@ -1302,10 +1502,14 @@
         <v>300</v>
       </c>
       <c r="D50" s="3">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
+        <v>19.444444599999997</v>
+      </c>
+      <c r="F50">
+        <f t="shared" si="0"/>
+        <v>5.4012346543209864</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A51" s="3" t="s">
         <v>20</v>
       </c>
@@ -1316,10 +1520,14 @@
         <v>15</v>
       </c>
       <c r="D51" s="3">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
+        <v>15.277777899999998</v>
+      </c>
+      <c r="F51">
+        <f t="shared" si="0"/>
+        <v>4.2438272283950615</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A52" s="3" t="s">
         <v>21</v>
       </c>
@@ -1330,10 +1538,14 @@
         <v>100</v>
       </c>
       <c r="D52" s="3">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
+        <v>16.666666799999998</v>
+      </c>
+      <c r="F52">
+        <f t="shared" si="0"/>
+        <v>4.6296297037037029</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A53" s="3" t="s">
         <v>21</v>
       </c>
@@ -1344,10 +1556,14 @@
         <v>100</v>
       </c>
       <c r="D53" s="3">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
+        <v>16.666666799999998</v>
+      </c>
+      <c r="F53">
+        <f t="shared" si="0"/>
+        <v>4.6296297037037029</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A54" s="3" t="s">
         <v>21</v>
       </c>
@@ -1358,10 +1574,14 @@
         <v>80</v>
       </c>
       <c r="D54" s="3">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
+        <v>16.666666799999998</v>
+      </c>
+      <c r="F54">
+        <f t="shared" si="0"/>
+        <v>4.6296297037037029</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A55" s="3" t="s">
         <v>22</v>
       </c>
@@ -1372,14 +1592,18 @@
         <v>100</v>
       </c>
       <c r="D55" s="3">
-        <v>60</v>
+        <v>16.666666799999998</v>
       </c>
       <c r="E55" s="5" t="str">
         <f>E14</f>
         <v>STATION; DORMONT</v>
       </c>
-    </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F55">
+        <f t="shared" si="0"/>
+        <v>4.6296297037037029</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A56" s="3" t="s">
         <v>22</v>
       </c>
@@ -1390,10 +1614,14 @@
         <v>100</v>
       </c>
       <c r="D56" s="3">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.3">
+        <v>16.666666799999998</v>
+      </c>
+      <c r="F56">
+        <f t="shared" si="0"/>
+        <v>4.6296297037037029</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A57" s="3" t="s">
         <v>22</v>
       </c>
@@ -1404,10 +1632,14 @@
         <v>90</v>
       </c>
       <c r="D57" s="3">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.3">
+        <v>16.666666799999998</v>
+      </c>
+      <c r="F57">
+        <f t="shared" si="0"/>
+        <v>4.6296297037037029</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A58" s="3" t="s">
         <v>22</v>
       </c>
@@ -1418,10 +1650,14 @@
         <v>100</v>
       </c>
       <c r="D58" s="3">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.3">
+        <v>16.666666799999998</v>
+      </c>
+      <c r="F58">
+        <f t="shared" si="0"/>
+        <v>4.6296297037037029</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A59" s="3" t="s">
         <v>22</v>
       </c>
@@ -1432,10 +1668,14 @@
         <v>100</v>
       </c>
       <c r="D59" s="3">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.3">
+        <v>16.666666799999998</v>
+      </c>
+      <c r="F59">
+        <f t="shared" si="0"/>
+        <v>4.6296297037037029</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A60" s="3" t="s">
         <v>23</v>
       </c>
@@ -1446,10 +1686,14 @@
         <v>100</v>
       </c>
       <c r="D60" s="3">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.3">
+        <v>19.444444599999997</v>
+      </c>
+      <c r="F60">
+        <f t="shared" si="0"/>
+        <v>5.4012346543209864</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A61" s="3" t="s">
         <v>23</v>
       </c>
@@ -1460,10 +1704,14 @@
         <v>100</v>
       </c>
       <c r="D61" s="3">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.3">
+        <v>19.444444599999997</v>
+      </c>
+      <c r="F61">
+        <f t="shared" si="0"/>
+        <v>5.4012346543209864</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A62" s="3" t="s">
         <v>23</v>
       </c>
@@ -1474,10 +1722,14 @@
         <v>100</v>
       </c>
       <c r="D62" s="3">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.3">
+        <v>19.444444599999997</v>
+      </c>
+      <c r="F62">
+        <f t="shared" si="0"/>
+        <v>5.4012346543209864</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A63" s="3" t="s">
         <v>23</v>
       </c>
@@ -1488,10 +1740,14 @@
         <v>100</v>
       </c>
       <c r="D63" s="3">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.3">
+        <v>19.444444599999997</v>
+      </c>
+      <c r="F63">
+        <f t="shared" si="0"/>
+        <v>5.4012346543209864</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A64" s="3" t="s">
         <v>23</v>
       </c>
@@ -1502,14 +1758,18 @@
         <v>100</v>
       </c>
       <c r="D64" s="3">
-        <v>70</v>
+        <v>19.444444599999997</v>
       </c>
       <c r="E64" s="5" t="str">
         <f>E6</f>
         <v>STATION; GLENBURY</v>
       </c>
-    </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F64">
+        <f t="shared" si="0"/>
+        <v>5.4012346543209864</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A65" s="3" t="s">
         <v>23</v>
       </c>
@@ -1520,10 +1780,14 @@
         <v>100</v>
       </c>
       <c r="D65" s="3">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.3">
+        <v>19.444444599999997</v>
+      </c>
+      <c r="F65">
+        <f t="shared" si="0"/>
+        <v>5.4012346543209864</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A66" s="3" t="s">
         <v>23</v>
       </c>
@@ -1534,10 +1798,14 @@
         <v>100</v>
       </c>
       <c r="D66" s="3">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.3">
+        <v>19.444444599999997</v>
+      </c>
+      <c r="F66">
+        <f t="shared" ref="F66:F129" si="1">D66*0.27777778</f>
+        <v>5.4012346543209864</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A67" s="3" t="s">
         <v>24</v>
       </c>
@@ -1548,10 +1816,14 @@
         <v>50</v>
       </c>
       <c r="D67" s="3">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.3">
+        <v>16.666666799999998</v>
+      </c>
+      <c r="F67">
+        <f t="shared" si="1"/>
+        <v>4.6296297037037029</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A68" s="3" t="s">
         <v>24</v>
       </c>
@@ -1562,10 +1834,14 @@
         <v>50</v>
       </c>
       <c r="D68" s="3">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.3">
+        <v>16.666666799999998</v>
+      </c>
+      <c r="F68">
+        <f t="shared" si="1"/>
+        <v>4.6296297037037029</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A69" s="3" t="s">
         <v>24</v>
       </c>
@@ -1576,10 +1852,14 @@
         <v>40</v>
       </c>
       <c r="D69" s="3">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.3">
+        <v>16.666666799999998</v>
+      </c>
+      <c r="F69">
+        <f t="shared" si="1"/>
+        <v>4.6296297037037029</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A70" s="3" t="s">
         <v>24</v>
       </c>
@@ -1590,10 +1870,14 @@
         <v>50</v>
       </c>
       <c r="D70" s="3">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.3">
+        <v>16.666666799999998</v>
+      </c>
+      <c r="F70">
+        <f t="shared" si="1"/>
+        <v>4.6296297037037029</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A71" s="3" t="s">
         <v>24</v>
       </c>
@@ -1604,10 +1888,14 @@
         <v>50</v>
       </c>
       <c r="D71" s="3">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.3">
+        <v>16.666666799999998</v>
+      </c>
+      <c r="F71">
+        <f t="shared" si="1"/>
+        <v>4.6296297037037029</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A72" s="3" t="s">
         <v>25</v>
       </c>
@@ -1618,13 +1906,17 @@
         <v>50</v>
       </c>
       <c r="D72" s="3">
-        <v>70</v>
+        <v>19.444444599999997</v>
       </c>
       <c r="E72" s="3" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="73" spans="1:5" ht="31.2" x14ac:dyDescent="0.3">
+        <v>32</v>
+      </c>
+      <c r="F72">
+        <f t="shared" si="1"/>
+        <v>5.4012346543209864</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A73" s="3" t="s">
         <v>25</v>
       </c>
@@ -1635,14 +1927,18 @@
         <v>50</v>
       </c>
       <c r="D73" s="3">
-        <v>70</v>
+        <v>19.444444599999997</v>
       </c>
       <c r="E73" s="5" t="str">
         <f>E173</f>
         <v>STATION; OVERBROOK; UNDERGROUND</v>
       </c>
-    </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F73">
+        <f t="shared" si="1"/>
+        <v>5.4012346543209864</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A74" s="3" t="s">
         <v>25</v>
       </c>
@@ -1653,13 +1949,17 @@
         <v>50</v>
       </c>
       <c r="D74" s="3">
-        <v>70</v>
+        <v>19.444444599999997</v>
       </c>
       <c r="E74" s="3" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.3">
+        <v>32</v>
+      </c>
+      <c r="F74">
+        <f t="shared" si="1"/>
+        <v>5.4012346543209864</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A75" s="3" t="s">
         <v>25</v>
       </c>
@@ -1670,13 +1970,17 @@
         <v>50</v>
       </c>
       <c r="D75" s="3">
-        <v>70</v>
+        <v>19.444444599999997</v>
       </c>
       <c r="E75" s="3" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.3">
+        <v>32</v>
+      </c>
+      <c r="F75">
+        <f t="shared" si="1"/>
+        <v>5.4012346543209864</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A76" s="3" t="s">
         <v>25</v>
       </c>
@@ -1687,13 +1991,17 @@
         <v>50</v>
       </c>
       <c r="D76" s="3">
-        <v>70</v>
+        <v>19.444444599999997</v>
       </c>
       <c r="E76" s="3" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.3">
+        <v>32</v>
+      </c>
+      <c r="F76">
+        <f t="shared" si="1"/>
+        <v>5.4012346543209864</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A77" s="3" t="s">
         <v>25</v>
       </c>
@@ -1704,13 +2012,17 @@
         <v>50</v>
       </c>
       <c r="D77" s="3">
-        <v>70</v>
+        <v>19.444444599999997</v>
       </c>
       <c r="E77" s="3" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.3">
+        <v>32</v>
+      </c>
+      <c r="F77">
+        <f t="shared" si="1"/>
+        <v>5.4012346543209864</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A78" s="3" t="s">
         <v>25</v>
       </c>
@@ -1721,13 +2033,17 @@
         <v>50</v>
       </c>
       <c r="D78" s="3">
-        <v>70</v>
+        <v>19.444444599999997</v>
       </c>
       <c r="E78" s="3" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.3">
+        <v>32</v>
+      </c>
+      <c r="F78">
+        <f t="shared" si="1"/>
+        <v>5.4012346543209864</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A79" s="3" t="s">
         <v>25</v>
       </c>
@@ -1738,13 +2054,17 @@
         <v>50</v>
       </c>
       <c r="D79" s="3">
-        <v>70</v>
+        <v>19.444444599999997</v>
       </c>
       <c r="E79" s="3" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.3">
+        <v>32</v>
+      </c>
+      <c r="F79">
+        <f t="shared" si="1"/>
+        <v>5.4012346543209864</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A80" s="3" t="s">
         <v>25</v>
       </c>
@@ -1755,13 +2075,17 @@
         <v>50</v>
       </c>
       <c r="D80" s="3">
-        <v>70</v>
+        <v>19.444444599999997</v>
       </c>
       <c r="E80" s="3" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.3">
+        <v>32</v>
+      </c>
+      <c r="F80">
+        <f t="shared" si="1"/>
+        <v>5.4012346543209864</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A81" s="3" t="s">
         <v>25</v>
       </c>
@@ -1772,13 +2096,17 @@
         <v>50</v>
       </c>
       <c r="D81" s="3">
-        <v>70</v>
+        <v>19.444444599999997</v>
       </c>
       <c r="E81" s="3" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="82" spans="1:5" ht="31.2" x14ac:dyDescent="0.3">
+        <v>32</v>
+      </c>
+      <c r="F81">
+        <f t="shared" si="1"/>
+        <v>5.4012346543209864</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A82" s="3" t="s">
         <v>25</v>
       </c>
@@ -1789,14 +2117,18 @@
         <v>50</v>
       </c>
       <c r="D82" s="3">
-        <v>70</v>
+        <v>19.444444599999997</v>
       </c>
       <c r="E82" s="5" t="str">
         <f>E164</f>
         <v>STATION; INGLEWOOD; UNDERGROUND</v>
       </c>
-    </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F82">
+        <f t="shared" si="1"/>
+        <v>5.4012346543209864</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A83" s="3" t="s">
         <v>25</v>
       </c>
@@ -1807,13 +2139,17 @@
         <v>50</v>
       </c>
       <c r="D83" s="3">
-        <v>70</v>
+        <v>19.444444599999997</v>
       </c>
       <c r="E83" s="3" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.3">
+        <v>32</v>
+      </c>
+      <c r="F83">
+        <f t="shared" si="1"/>
+        <v>5.4012346543209864</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A84" s="3" t="s">
         <v>25</v>
       </c>
@@ -1824,13 +2160,17 @@
         <v>50</v>
       </c>
       <c r="D84" s="3">
-        <v>70</v>
+        <v>19.444444599999997</v>
       </c>
       <c r="E84" s="3" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.3">
+        <v>32</v>
+      </c>
+      <c r="F84">
+        <f t="shared" si="1"/>
+        <v>5.4012346543209864</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A85" s="3" t="s">
         <v>25</v>
       </c>
@@ -1841,13 +2181,17 @@
         <v>50</v>
       </c>
       <c r="D85" s="3">
-        <v>70</v>
+        <v>19.444444599999997</v>
       </c>
       <c r="E85" s="3" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.3">
+        <v>32</v>
+      </c>
+      <c r="F85">
+        <f t="shared" si="1"/>
+        <v>5.4012346543209864</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A86" s="3" t="s">
         <v>25</v>
       </c>
@@ -1858,13 +2202,17 @@
         <v>50</v>
       </c>
       <c r="D86" s="3">
-        <v>70</v>
+        <v>19.444444599999997</v>
       </c>
       <c r="E86" s="3" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.3">
+        <v>32</v>
+      </c>
+      <c r="F86">
+        <f t="shared" si="1"/>
+        <v>5.4012346543209864</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A87" s="3" t="s">
         <v>25</v>
       </c>
@@ -1875,13 +2223,17 @@
         <v>50</v>
       </c>
       <c r="D87" s="3">
-        <v>70</v>
+        <v>19.444444599999997</v>
       </c>
       <c r="E87" s="3" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.3">
+        <v>32</v>
+      </c>
+      <c r="F87">
+        <f t="shared" si="1"/>
+        <v>5.4012346543209864</v>
+      </c>
+    </row>
+    <row r="88" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A88" s="3" t="s">
         <v>25</v>
       </c>
@@ -1892,13 +2244,17 @@
         <v>50</v>
       </c>
       <c r="D88" s="3">
-        <v>70</v>
+        <v>19.444444599999997</v>
       </c>
       <c r="E88" s="3" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.3">
+        <v>32</v>
+      </c>
+      <c r="F88">
+        <f t="shared" si="1"/>
+        <v>5.4012346543209864</v>
+      </c>
+    </row>
+    <row r="89" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A89" s="3" t="s">
         <v>25</v>
       </c>
@@ -1909,13 +2265,17 @@
         <v>50</v>
       </c>
       <c r="D89" s="3">
-        <v>70</v>
+        <v>19.444444599999997</v>
       </c>
       <c r="E89" s="3" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.3">
+        <v>32</v>
+      </c>
+      <c r="F89">
+        <f t="shared" si="1"/>
+        <v>5.4012346543209864</v>
+      </c>
+    </row>
+    <row r="90" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A90" s="3" t="s">
         <v>25</v>
       </c>
@@ -1926,13 +2286,17 @@
         <v>50</v>
       </c>
       <c r="D90" s="3">
-        <v>70</v>
+        <v>19.444444599999997</v>
       </c>
       <c r="E90" s="3" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.3">
+        <v>32</v>
+      </c>
+      <c r="F90">
+        <f t="shared" si="1"/>
+        <v>5.4012346543209864</v>
+      </c>
+    </row>
+    <row r="91" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A91" s="3" t="s">
         <v>25</v>
       </c>
@@ -1943,14 +2307,18 @@
         <v>50</v>
       </c>
       <c r="D91" s="3">
-        <v>70</v>
+        <v>19.444444599999997</v>
       </c>
       <c r="E91" s="5" t="str">
         <f>E155</f>
         <v>STATION; CENTRAL; UNDERGROUND</v>
       </c>
-    </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F91">
+        <f t="shared" si="1"/>
+        <v>5.4012346543209864</v>
+      </c>
+    </row>
+    <row r="92" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A92" s="3" t="s">
         <v>25</v>
       </c>
@@ -1961,13 +2329,17 @@
         <v>50</v>
       </c>
       <c r="D92" s="3">
-        <v>70</v>
+        <v>19.444444599999997</v>
       </c>
       <c r="E92" s="5" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.3">
+        <v>32</v>
+      </c>
+      <c r="F92">
+        <f t="shared" si="1"/>
+        <v>5.4012346543209864</v>
+      </c>
+    </row>
+    <row r="93" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A93" s="3" t="s">
         <v>25</v>
       </c>
@@ -1978,15 +2350,19 @@
         <v>50</v>
       </c>
       <c r="D93" s="3">
-        <v>70</v>
+        <v>19.444444599999997</v>
       </c>
       <c r="E93" s="5" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.3">
+        <v>32</v>
+      </c>
+      <c r="F93">
+        <f t="shared" si="1"/>
+        <v>5.4012346543209864</v>
+      </c>
+    </row>
+    <row r="94" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A94" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B94" s="3">
         <v>144</v>
@@ -1995,13 +2371,17 @@
         <v>50</v>
       </c>
       <c r="D94" s="3">
-        <v>70</v>
+        <v>19.444444599999997</v>
       </c>
       <c r="E94" s="5"/>
-    </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F94">
+        <f t="shared" si="1"/>
+        <v>5.4012346543209864</v>
+      </c>
+    </row>
+    <row r="95" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A95" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B95" s="3">
         <v>145</v>
@@ -2010,13 +2390,17 @@
         <v>50</v>
       </c>
       <c r="D95" s="3">
-        <v>70</v>
+        <v>19.444444599999997</v>
       </c>
       <c r="E95" s="5"/>
-    </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F95">
+        <f t="shared" si="1"/>
+        <v>5.4012346543209864</v>
+      </c>
+    </row>
+    <row r="96" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A96" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B96" s="3">
         <v>146</v>
@@ -2025,13 +2409,17 @@
         <v>50</v>
       </c>
       <c r="D96" s="3">
-        <v>70</v>
+        <v>19.444444599999997</v>
       </c>
       <c r="E96" s="5"/>
-    </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F96">
+        <f t="shared" si="1"/>
+        <v>5.4012346543209864</v>
+      </c>
+    </row>
+    <row r="97" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A97" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B97" s="3">
         <v>147</v>
@@ -2040,13 +2428,17 @@
         <v>50</v>
       </c>
       <c r="D97" s="3">
-        <v>70</v>
+        <v>19.444444599999997</v>
       </c>
       <c r="E97" s="5"/>
-    </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F97">
+        <f t="shared" si="1"/>
+        <v>5.4012346543209864</v>
+      </c>
+    </row>
+    <row r="98" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A98" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B98" s="3">
         <v>148</v>
@@ -2055,13 +2447,17 @@
         <v>184</v>
       </c>
       <c r="D98" s="3">
-        <v>70</v>
+        <v>19.444444599999997</v>
       </c>
       <c r="E98" s="5"/>
-    </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F98">
+        <f t="shared" si="1"/>
+        <v>5.4012346543209864</v>
+      </c>
+    </row>
+    <row r="99" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A99" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B99" s="3">
         <v>149</v>
@@ -2070,13 +2466,17 @@
         <v>40</v>
       </c>
       <c r="D99" s="3">
-        <v>70</v>
+        <v>19.444444599999997</v>
       </c>
       <c r="E99" s="5"/>
-    </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F99">
+        <f t="shared" si="1"/>
+        <v>5.4012346543209864</v>
+      </c>
+    </row>
+    <row r="100" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A100" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B100" s="3">
         <v>150</v>
@@ -2085,11 +2485,15 @@
         <v>35</v>
       </c>
       <c r="D100" s="3">
-        <v>70</v>
+        <v>19.444444599999997</v>
       </c>
       <c r="E100" s="5"/>
-    </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F100">
+        <f t="shared" si="1"/>
+        <v>5.4012346543209864</v>
+      </c>
+    </row>
+    <row r="101" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A101" s="3" t="s">
         <v>8</v>
       </c>
@@ -2100,11 +2504,15 @@
         <v>50</v>
       </c>
       <c r="D101" s="3">
-        <v>70</v>
+        <v>19.444444599999997</v>
       </c>
       <c r="E101" s="5"/>
-    </row>
-    <row r="102" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F101">
+        <f t="shared" si="1"/>
+        <v>5.4012346543209864</v>
+      </c>
+    </row>
+    <row r="102" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A102" s="3" t="s">
         <v>8</v>
       </c>
@@ -2115,11 +2523,15 @@
         <v>50</v>
       </c>
       <c r="D102" s="3">
-        <v>70</v>
+        <v>19.444444599999997</v>
       </c>
       <c r="E102" s="5"/>
-    </row>
-    <row r="103" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F102">
+        <f t="shared" si="1"/>
+        <v>5.4012346543209864</v>
+      </c>
+    </row>
+    <row r="103" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A103" s="3" t="s">
         <v>8</v>
       </c>
@@ -2130,11 +2542,15 @@
         <v>100</v>
       </c>
       <c r="D103" s="3">
-        <v>70</v>
+        <v>19.444444599999997</v>
       </c>
       <c r="E103" s="5"/>
-    </row>
-    <row r="104" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F103">
+        <f t="shared" si="1"/>
+        <v>5.4012346543209864</v>
+      </c>
+    </row>
+    <row r="104" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A104" s="3" t="s">
         <v>8</v>
       </c>
@@ -2145,10 +2561,14 @@
         <v>200</v>
       </c>
       <c r="D104" s="3">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="105" spans="1:5" x14ac:dyDescent="0.3">
+        <v>19.444444599999997</v>
+      </c>
+      <c r="F104">
+        <f t="shared" si="1"/>
+        <v>5.4012346543209864</v>
+      </c>
+    </row>
+    <row r="105" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A105" s="3" t="s">
         <v>8</v>
       </c>
@@ -2159,10 +2579,14 @@
         <v>300</v>
       </c>
       <c r="D105" s="3">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="106" spans="1:5" x14ac:dyDescent="0.3">
+        <v>19.444444599999997</v>
+      </c>
+      <c r="F105">
+        <f t="shared" si="1"/>
+        <v>5.4012346543209864</v>
+      </c>
+    </row>
+    <row r="106" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A106" s="3" t="s">
         <v>8</v>
       </c>
@@ -2173,10 +2597,14 @@
         <v>300</v>
       </c>
       <c r="D106" s="3">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="107" spans="1:5" x14ac:dyDescent="0.3">
+        <v>19.444444599999997</v>
+      </c>
+      <c r="F106">
+        <f t="shared" si="1"/>
+        <v>5.4012346543209864</v>
+      </c>
+    </row>
+    <row r="107" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A107" s="3" t="s">
         <v>8</v>
       </c>
@@ -2187,13 +2615,17 @@
         <v>300</v>
       </c>
       <c r="D107" s="3">
-        <v>70</v>
+        <v>19.444444599999997</v>
       </c>
       <c r="E107" s="5" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="108" spans="1:5" x14ac:dyDescent="0.3">
+        <v>30</v>
+      </c>
+      <c r="F107">
+        <f t="shared" si="1"/>
+        <v>5.4012346543209864</v>
+      </c>
+    </row>
+    <row r="108" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A108" s="3" t="s">
         <v>8</v>
       </c>
@@ -2204,10 +2636,14 @@
         <v>300</v>
       </c>
       <c r="D108" s="3">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="109" spans="1:5" x14ac:dyDescent="0.3">
+        <v>19.444444599999997</v>
+      </c>
+      <c r="F108">
+        <f t="shared" si="1"/>
+        <v>5.4012346543209864</v>
+      </c>
+    </row>
+    <row r="109" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A109" s="3" t="s">
         <v>7</v>
       </c>
@@ -2218,10 +2654,14 @@
         <v>150</v>
       </c>
       <c r="D109" s="3">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="110" spans="1:5" x14ac:dyDescent="0.3">
+        <v>16.666666799999998</v>
+      </c>
+      <c r="F109">
+        <f t="shared" si="1"/>
+        <v>4.6296297037037029</v>
+      </c>
+    </row>
+    <row r="110" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A110" s="3" t="s">
         <v>7</v>
       </c>
@@ -2232,10 +2672,14 @@
         <v>150</v>
       </c>
       <c r="D110" s="3">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="111" spans="1:5" x14ac:dyDescent="0.3">
+        <v>16.666666799999998</v>
+      </c>
+      <c r="F110">
+        <f t="shared" si="1"/>
+        <v>4.6296297037037029</v>
+      </c>
+    </row>
+    <row r="111" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A111" s="3" t="s">
         <v>7</v>
       </c>
@@ -2246,10 +2690,14 @@
         <v>150</v>
       </c>
       <c r="D111" s="3">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="112" spans="1:5" x14ac:dyDescent="0.3">
+        <v>16.666666799999998</v>
+      </c>
+      <c r="F111">
+        <f t="shared" si="1"/>
+        <v>4.6296297037037029</v>
+      </c>
+    </row>
+    <row r="112" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A112" s="3" t="s">
         <v>7</v>
       </c>
@@ -2260,10 +2708,14 @@
         <v>150</v>
       </c>
       <c r="D112" s="3">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="113" spans="1:5" x14ac:dyDescent="0.3">
+        <v>16.666666799999998</v>
+      </c>
+      <c r="F112">
+        <f t="shared" si="1"/>
+        <v>4.6296297037037029</v>
+      </c>
+    </row>
+    <row r="113" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A113" s="3" t="s">
         <v>6</v>
       </c>
@@ -2274,13 +2726,17 @@
         <v>150</v>
       </c>
       <c r="D113" s="3">
-        <v>70</v>
+        <v>19.444444599999997</v>
       </c>
       <c r="E113" s="5" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="114" spans="1:5" x14ac:dyDescent="0.3">
+        <v>44</v>
+      </c>
+      <c r="F113">
+        <f t="shared" si="1"/>
+        <v>5.4012346543209864</v>
+      </c>
+    </row>
+    <row r="114" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A114" s="3" t="s">
         <v>6</v>
       </c>
@@ -2291,10 +2747,14 @@
         <v>150</v>
       </c>
       <c r="D114" s="3">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="115" spans="1:5" x14ac:dyDescent="0.3">
+        <v>19.444444599999997</v>
+      </c>
+      <c r="F114">
+        <f t="shared" si="1"/>
+        <v>5.4012346543209864</v>
+      </c>
+    </row>
+    <row r="115" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A115" s="3" t="s">
         <v>6</v>
       </c>
@@ -2305,10 +2765,14 @@
         <v>150</v>
       </c>
       <c r="D115" s="3">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="116" spans="1:5" x14ac:dyDescent="0.3">
+        <v>19.444444599999997</v>
+      </c>
+      <c r="F115">
+        <f t="shared" si="1"/>
+        <v>5.4012346543209864</v>
+      </c>
+    </row>
+    <row r="116" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A116" s="3" t="s">
         <v>6</v>
       </c>
@@ -2319,10 +2783,14 @@
         <v>150</v>
       </c>
       <c r="D116" s="3">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="117" spans="1:5" x14ac:dyDescent="0.3">
+        <v>19.444444599999997</v>
+      </c>
+      <c r="F116">
+        <f t="shared" si="1"/>
+        <v>5.4012346543209864</v>
+      </c>
+    </row>
+    <row r="117" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A117" s="3" t="s">
         <v>5</v>
       </c>
@@ -2333,13 +2801,17 @@
         <v>100</v>
       </c>
       <c r="D117" s="3">
-        <v>55</v>
+        <v>15.277777899999998</v>
       </c>
       <c r="E117" s="3" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="118" spans="1:5" x14ac:dyDescent="0.3">
+        <v>29</v>
+      </c>
+      <c r="F117">
+        <f t="shared" si="1"/>
+        <v>4.2438272283950615</v>
+      </c>
+    </row>
+    <row r="118" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A118" s="3" t="s">
         <v>5</v>
       </c>
@@ -2350,10 +2822,14 @@
         <v>100</v>
       </c>
       <c r="D118" s="3">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="119" spans="1:5" x14ac:dyDescent="0.3">
+        <v>15.277777899999998</v>
+      </c>
+      <c r="F118">
+        <f t="shared" si="1"/>
+        <v>4.2438272283950615</v>
+      </c>
+    </row>
+    <row r="119" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A119" s="3" t="s">
         <v>5</v>
       </c>
@@ -2364,10 +2840,14 @@
         <v>100</v>
       </c>
       <c r="D119" s="3">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="120" spans="1:5" x14ac:dyDescent="0.3">
+        <v>15.277777899999998</v>
+      </c>
+      <c r="F119">
+        <f t="shared" si="1"/>
+        <v>4.2438272283950615</v>
+      </c>
+    </row>
+    <row r="120" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A120" s="3" t="s">
         <v>5</v>
       </c>
@@ -2378,13 +2858,17 @@
         <v>100</v>
       </c>
       <c r="D120" s="3">
-        <v>55</v>
+        <v>15.277777899999998</v>
       </c>
       <c r="E120" s="5" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="121" spans="1:5" x14ac:dyDescent="0.3">
+        <v>28</v>
+      </c>
+      <c r="F120">
+        <f t="shared" si="1"/>
+        <v>4.2438272283950615</v>
+      </c>
+    </row>
+    <row r="121" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A121" s="3" t="s">
         <v>5</v>
       </c>
@@ -2395,10 +2879,14 @@
         <v>100</v>
       </c>
       <c r="D121" s="3">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="122" spans="1:5" x14ac:dyDescent="0.3">
+        <v>15.277777899999998</v>
+      </c>
+      <c r="F121">
+        <f t="shared" si="1"/>
+        <v>4.2438272283950615</v>
+      </c>
+    </row>
+    <row r="122" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A122" s="3" t="s">
         <v>5</v>
       </c>
@@ -2409,10 +2897,14 @@
         <v>100</v>
       </c>
       <c r="D122" s="3">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="123" spans="1:5" x14ac:dyDescent="0.3">
+        <v>15.277777899999998</v>
+      </c>
+      <c r="F122">
+        <f t="shared" si="1"/>
+        <v>4.2438272283950615</v>
+      </c>
+    </row>
+    <row r="123" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A123" s="3" t="s">
         <v>4</v>
       </c>
@@ -2423,10 +2915,14 @@
         <v>100</v>
       </c>
       <c r="D123" s="3">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="124" spans="1:5" x14ac:dyDescent="0.3">
+        <v>15.277777899999998</v>
+      </c>
+      <c r="F123">
+        <f t="shared" si="1"/>
+        <v>4.2438272283950615</v>
+      </c>
+    </row>
+    <row r="124" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A124" s="3" t="s">
         <v>4</v>
       </c>
@@ -2437,10 +2933,14 @@
         <v>100</v>
       </c>
       <c r="D124" s="3">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="125" spans="1:5" x14ac:dyDescent="0.3">
+        <v>15.277777899999998</v>
+      </c>
+      <c r="F124">
+        <f t="shared" si="1"/>
+        <v>4.2438272283950615</v>
+      </c>
+    </row>
+    <row r="125" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A125" s="3" t="s">
         <v>4</v>
       </c>
@@ -2451,10 +2951,14 @@
         <v>100</v>
       </c>
       <c r="D125" s="3">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="126" spans="1:5" x14ac:dyDescent="0.3">
+        <v>15.277777899999998</v>
+      </c>
+      <c r="F125">
+        <f t="shared" si="1"/>
+        <v>4.2438272283950615</v>
+      </c>
+    </row>
+    <row r="126" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A126" s="3" t="s">
         <v>3</v>
       </c>
@@ -2465,10 +2969,14 @@
         <v>100</v>
       </c>
       <c r="D126" s="3">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="127" spans="1:5" x14ac:dyDescent="0.3">
+        <v>15.277777899999998</v>
+      </c>
+      <c r="F126">
+        <f t="shared" si="1"/>
+        <v>4.2438272283950615</v>
+      </c>
+    </row>
+    <row r="127" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A127" s="3" t="s">
         <v>3</v>
       </c>
@@ -2479,13 +2987,17 @@
         <v>100</v>
       </c>
       <c r="D127" s="3">
-        <v>55</v>
+        <v>15.277777899999998</v>
       </c>
       <c r="E127" s="5" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="128" spans="1:5" x14ac:dyDescent="0.3">
+        <v>27</v>
+      </c>
+      <c r="F127">
+        <f t="shared" si="1"/>
+        <v>4.2438272283950615</v>
+      </c>
+    </row>
+    <row r="128" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A128" s="3" t="s">
         <v>3</v>
       </c>
@@ -2496,10 +3008,14 @@
         <v>100</v>
       </c>
       <c r="D128" s="3">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="129" spans="1:5" x14ac:dyDescent="0.3">
+        <v>15.277777899999998</v>
+      </c>
+      <c r="F128">
+        <f t="shared" si="1"/>
+        <v>4.2438272283950615</v>
+      </c>
+    </row>
+    <row r="129" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A129" s="3" t="s">
         <v>6</v>
       </c>
@@ -2510,10 +3026,14 @@
         <v>150</v>
       </c>
       <c r="D129" s="3">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="130" spans="1:5" x14ac:dyDescent="0.3">
+        <v>19.444444599999997</v>
+      </c>
+      <c r="F129">
+        <f t="shared" si="1"/>
+        <v>5.4012346543209864</v>
+      </c>
+    </row>
+    <row r="130" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A130" s="3" t="s">
         <v>6</v>
       </c>
@@ -2524,10 +3044,14 @@
         <v>150</v>
       </c>
       <c r="D130" s="3">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="131" spans="1:5" x14ac:dyDescent="0.3">
+        <v>19.444444599999997</v>
+      </c>
+      <c r="F130">
+        <f t="shared" ref="F130:F178" si="2">D130*0.27777778</f>
+        <v>5.4012346543209864</v>
+      </c>
+    </row>
+    <row r="131" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A131" s="3" t="s">
         <v>6</v>
       </c>
@@ -2538,10 +3062,14 @@
         <v>150</v>
       </c>
       <c r="D131" s="3">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="132" spans="1:5" x14ac:dyDescent="0.3">
+        <v>19.444444599999997</v>
+      </c>
+      <c r="F131">
+        <f t="shared" si="2"/>
+        <v>5.4012346543209864</v>
+      </c>
+    </row>
+    <row r="132" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A132" s="3" t="s">
         <v>6</v>
       </c>
@@ -2552,13 +3080,17 @@
         <v>150</v>
       </c>
       <c r="D132" s="3">
-        <v>70</v>
+        <v>19.444444599999997</v>
       </c>
       <c r="E132" s="5" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="133" spans="1:5" x14ac:dyDescent="0.3">
+        <v>44</v>
+      </c>
+      <c r="F132">
+        <f t="shared" si="2"/>
+        <v>5.4012346543209864</v>
+      </c>
+    </row>
+    <row r="133" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A133" s="3" t="s">
         <v>7</v>
       </c>
@@ -2569,10 +3101,14 @@
         <v>150</v>
       </c>
       <c r="D133" s="3">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="134" spans="1:5" x14ac:dyDescent="0.3">
+        <v>16.666666799999998</v>
+      </c>
+      <c r="F133">
+        <f t="shared" si="2"/>
+        <v>4.6296297037037029</v>
+      </c>
+    </row>
+    <row r="134" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A134" s="3" t="s">
         <v>7</v>
       </c>
@@ -2583,10 +3119,14 @@
         <v>150</v>
       </c>
       <c r="D134" s="3">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="135" spans="1:5" x14ac:dyDescent="0.3">
+        <v>16.666666799999998</v>
+      </c>
+      <c r="F134">
+        <f t="shared" si="2"/>
+        <v>4.6296297037037029</v>
+      </c>
+    </row>
+    <row r="135" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A135" s="3" t="s">
         <v>7</v>
       </c>
@@ -2597,10 +3137,14 @@
         <v>150</v>
       </c>
       <c r="D135" s="3">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="136" spans="1:5" x14ac:dyDescent="0.3">
+        <v>16.666666799999998</v>
+      </c>
+      <c r="F135">
+        <f t="shared" si="2"/>
+        <v>4.6296297037037029</v>
+      </c>
+    </row>
+    <row r="136" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A136" s="3" t="s">
         <v>7</v>
       </c>
@@ -2611,10 +3155,14 @@
         <v>150</v>
       </c>
       <c r="D136" s="3">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="137" spans="1:5" x14ac:dyDescent="0.3">
+        <v>16.666666799999998</v>
+      </c>
+      <c r="F136">
+        <f t="shared" si="2"/>
+        <v>4.6296297037037029</v>
+      </c>
+    </row>
+    <row r="137" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A137" s="3" t="s">
         <v>8</v>
       </c>
@@ -2625,10 +3173,14 @@
         <v>300</v>
       </c>
       <c r="D137" s="3">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="138" spans="1:5" x14ac:dyDescent="0.3">
+        <v>19.444444599999997</v>
+      </c>
+      <c r="F137">
+        <f t="shared" si="2"/>
+        <v>5.4012346543209864</v>
+      </c>
+    </row>
+    <row r="138" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A138" s="3" t="s">
         <v>8</v>
       </c>
@@ -2639,10 +3191,14 @@
         <v>300</v>
       </c>
       <c r="D138" s="3">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="139" spans="1:5" x14ac:dyDescent="0.3">
+        <v>19.444444599999997</v>
+      </c>
+      <c r="F138">
+        <f t="shared" si="2"/>
+        <v>5.4012346543209864</v>
+      </c>
+    </row>
+    <row r="139" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A139" s="3" t="s">
         <v>8</v>
       </c>
@@ -2653,10 +3209,14 @@
         <v>300</v>
       </c>
       <c r="D139" s="3">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="140" spans="1:5" x14ac:dyDescent="0.3">
+        <v>19.444444599999997</v>
+      </c>
+      <c r="F139">
+        <f t="shared" si="2"/>
+        <v>5.4012346543209864</v>
+      </c>
+    </row>
+    <row r="140" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A140" s="3" t="s">
         <v>8</v>
       </c>
@@ -2667,10 +3227,14 @@
         <v>300</v>
       </c>
       <c r="D140" s="3">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="141" spans="1:5" x14ac:dyDescent="0.3">
+        <v>19.444444599999997</v>
+      </c>
+      <c r="F140">
+        <f t="shared" si="2"/>
+        <v>5.4012346543209864</v>
+      </c>
+    </row>
+    <row r="141" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A141" s="3" t="s">
         <v>8</v>
       </c>
@@ -2681,10 +3245,14 @@
         <v>200</v>
       </c>
       <c r="D141" s="3">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="142" spans="1:5" x14ac:dyDescent="0.3">
+        <v>19.444444599999997</v>
+      </c>
+      <c r="F141">
+        <f t="shared" si="2"/>
+        <v>5.4012346543209864</v>
+      </c>
+    </row>
+    <row r="142" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A142" s="3" t="s">
         <v>8</v>
       </c>
@@ -2695,10 +3263,14 @@
         <v>100</v>
       </c>
       <c r="D142" s="3">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="143" spans="1:5" x14ac:dyDescent="0.3">
+        <v>19.444444599999997</v>
+      </c>
+      <c r="F142">
+        <f t="shared" si="2"/>
+        <v>5.4012346543209864</v>
+      </c>
+    </row>
+    <row r="143" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A143" s="3" t="s">
         <v>8</v>
       </c>
@@ -2709,10 +3281,14 @@
         <v>50</v>
       </c>
       <c r="D143" s="3">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="144" spans="1:5" x14ac:dyDescent="0.3">
+        <v>19.444444599999997</v>
+      </c>
+      <c r="F143">
+        <f t="shared" si="2"/>
+        <v>5.4012346543209864</v>
+      </c>
+    </row>
+    <row r="144" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A144" s="3" t="s">
         <v>8</v>
       </c>
@@ -2723,10 +3299,14 @@
         <v>50</v>
       </c>
       <c r="D144" s="3">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="145" spans="1:5" x14ac:dyDescent="0.3">
+        <v>19.444444599999997</v>
+      </c>
+      <c r="F144">
+        <f t="shared" si="2"/>
+        <v>5.4012346543209864</v>
+      </c>
+    </row>
+    <row r="145" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A145" s="3" t="s">
         <v>9</v>
       </c>
@@ -2737,13 +3317,17 @@
         <v>50</v>
       </c>
       <c r="D145" s="3">
-        <v>70</v>
+        <v>19.444444599999997</v>
       </c>
       <c r="E145" s="3" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="146" spans="1:5" x14ac:dyDescent="0.3">
+        <v>29</v>
+      </c>
+      <c r="F145">
+        <f t="shared" si="2"/>
+        <v>5.4012346543209864</v>
+      </c>
+    </row>
+    <row r="146" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A146" s="3" t="s">
         <v>9</v>
       </c>
@@ -2754,10 +3338,14 @@
         <v>50</v>
       </c>
       <c r="D146" s="3">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="147" spans="1:5" x14ac:dyDescent="0.3">
+        <v>19.444444599999997</v>
+      </c>
+      <c r="F146">
+        <f t="shared" si="2"/>
+        <v>5.4012346543209864</v>
+      </c>
+    </row>
+    <row r="147" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A147" s="3" t="s">
         <v>9</v>
       </c>
@@ -2768,13 +3356,17 @@
         <v>50</v>
       </c>
       <c r="D147" s="3">
-        <v>70</v>
+        <v>19.444444599999997</v>
       </c>
       <c r="E147" s="5" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="148" spans="1:5" x14ac:dyDescent="0.3">
+        <v>31</v>
+      </c>
+      <c r="F147">
+        <f t="shared" si="2"/>
+        <v>5.4012346543209864</v>
+      </c>
+    </row>
+    <row r="148" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A148" s="3" t="s">
         <v>9</v>
       </c>
@@ -2785,10 +3377,14 @@
         <v>50</v>
       </c>
       <c r="D148" s="3">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="149" spans="1:5" x14ac:dyDescent="0.3">
+        <v>19.444444599999997</v>
+      </c>
+      <c r="F148">
+        <f t="shared" si="2"/>
+        <v>5.4012346543209864</v>
+      </c>
+    </row>
+    <row r="149" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A149" s="3" t="s">
         <v>10</v>
       </c>
@@ -2799,10 +3395,14 @@
         <v>50</v>
       </c>
       <c r="D149" s="3">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="150" spans="1:5" x14ac:dyDescent="0.3">
+        <v>19.444444599999997</v>
+      </c>
+      <c r="F149">
+        <f t="shared" si="2"/>
+        <v>5.4012346543209864</v>
+      </c>
+    </row>
+    <row r="150" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A150" s="3" t="s">
         <v>10</v>
       </c>
@@ -2813,10 +3413,14 @@
         <v>50</v>
       </c>
       <c r="D150" s="3">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="151" spans="1:5" x14ac:dyDescent="0.3">
+        <v>19.444444599999997</v>
+      </c>
+      <c r="F150">
+        <f t="shared" si="2"/>
+        <v>5.4012346543209864</v>
+      </c>
+    </row>
+    <row r="151" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A151" s="3" t="s">
         <v>10</v>
       </c>
@@ -2827,10 +3431,14 @@
         <v>50</v>
       </c>
       <c r="D151" s="3">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="152" spans="1:5" x14ac:dyDescent="0.3">
+        <v>19.444444599999997</v>
+      </c>
+      <c r="F151">
+        <f t="shared" si="2"/>
+        <v>5.4012346543209864</v>
+      </c>
+    </row>
+    <row r="152" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A152" s="3" t="s">
         <v>11</v>
       </c>
@@ -2841,13 +3449,17 @@
         <v>50</v>
       </c>
       <c r="D152" s="3">
-        <v>70</v>
+        <v>19.444444599999997</v>
       </c>
       <c r="E152" s="3" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="153" spans="1:5" x14ac:dyDescent="0.3">
+        <v>32</v>
+      </c>
+      <c r="F152">
+        <f t="shared" si="2"/>
+        <v>5.4012346543209864</v>
+      </c>
+    </row>
+    <row r="153" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A153" s="3" t="s">
         <v>11</v>
       </c>
@@ -2858,13 +3470,17 @@
         <v>50</v>
       </c>
       <c r="D153" s="3">
-        <v>70</v>
+        <v>19.444444599999997</v>
       </c>
       <c r="E153" s="3" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="154" spans="1:5" x14ac:dyDescent="0.3">
+        <v>32</v>
+      </c>
+      <c r="F153">
+        <f t="shared" si="2"/>
+        <v>5.4012346543209864</v>
+      </c>
+    </row>
+    <row r="154" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A154" s="3" t="s">
         <v>11</v>
       </c>
@@ -2875,13 +3491,17 @@
         <v>50</v>
       </c>
       <c r="D154" s="3">
-        <v>70</v>
+        <v>19.444444599999997</v>
       </c>
       <c r="E154" s="3" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="155" spans="1:5" x14ac:dyDescent="0.3">
+        <v>32</v>
+      </c>
+      <c r="F154">
+        <f t="shared" si="2"/>
+        <v>5.4012346543209864</v>
+      </c>
+    </row>
+    <row r="155" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A155" s="3" t="s">
         <v>11</v>
       </c>
@@ -2892,13 +3512,17 @@
         <v>50</v>
       </c>
       <c r="D155" s="3">
-        <v>70</v>
+        <v>19.444444599999997</v>
       </c>
       <c r="E155" s="5" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="156" spans="1:5" x14ac:dyDescent="0.3">
+        <v>42</v>
+      </c>
+      <c r="F155">
+        <f t="shared" si="2"/>
+        <v>5.4012346543209864</v>
+      </c>
+    </row>
+    <row r="156" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A156" s="3" t="s">
         <v>11</v>
       </c>
@@ -2909,13 +3533,17 @@
         <v>50</v>
       </c>
       <c r="D156" s="3">
-        <v>70</v>
+        <v>19.444444599999997</v>
       </c>
       <c r="E156" s="3" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="157" spans="1:5" x14ac:dyDescent="0.3">
+        <v>32</v>
+      </c>
+      <c r="F156">
+        <f t="shared" si="2"/>
+        <v>5.4012346543209864</v>
+      </c>
+    </row>
+    <row r="157" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A157" s="3" t="s">
         <v>11</v>
       </c>
@@ -2926,13 +3554,17 @@
         <v>50</v>
       </c>
       <c r="D157" s="3">
-        <v>70</v>
+        <v>19.444444599999997</v>
       </c>
       <c r="E157" s="3" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="158" spans="1:5" x14ac:dyDescent="0.3">
+        <v>32</v>
+      </c>
+      <c r="F157">
+        <f t="shared" si="2"/>
+        <v>5.4012346543209864</v>
+      </c>
+    </row>
+    <row r="158" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A158" s="3" t="s">
         <v>11</v>
       </c>
@@ -2943,13 +3575,17 @@
         <v>50</v>
       </c>
       <c r="D158" s="3">
-        <v>70</v>
+        <v>19.444444599999997</v>
       </c>
       <c r="E158" s="3" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="159" spans="1:5" x14ac:dyDescent="0.3">
+        <v>32</v>
+      </c>
+      <c r="F158">
+        <f t="shared" si="2"/>
+        <v>5.4012346543209864</v>
+      </c>
+    </row>
+    <row r="159" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A159" s="3" t="s">
         <v>11</v>
       </c>
@@ -2960,13 +3596,17 @@
         <v>50</v>
       </c>
       <c r="D159" s="3">
-        <v>70</v>
+        <v>19.444444599999997</v>
       </c>
       <c r="E159" s="3" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="160" spans="1:5" x14ac:dyDescent="0.3">
+        <v>32</v>
+      </c>
+      <c r="F159">
+        <f t="shared" si="2"/>
+        <v>5.4012346543209864</v>
+      </c>
+    </row>
+    <row r="160" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A160" s="3" t="s">
         <v>11</v>
       </c>
@@ -2977,13 +3617,17 @@
         <v>50</v>
       </c>
       <c r="D160" s="3">
-        <v>70</v>
+        <v>19.444444599999997</v>
       </c>
       <c r="E160" s="3" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="161" spans="1:5" x14ac:dyDescent="0.3">
+        <v>32</v>
+      </c>
+      <c r="F160">
+        <f t="shared" si="2"/>
+        <v>5.4012346543209864</v>
+      </c>
+    </row>
+    <row r="161" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A161" s="3" t="s">
         <v>11</v>
       </c>
@@ -2994,13 +3638,17 @@
         <v>50</v>
       </c>
       <c r="D161" s="3">
-        <v>70</v>
+        <v>19.444444599999997</v>
       </c>
       <c r="E161" s="3" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="162" spans="1:5" x14ac:dyDescent="0.3">
+        <v>32</v>
+      </c>
+      <c r="F161">
+        <f t="shared" si="2"/>
+        <v>5.4012346543209864</v>
+      </c>
+    </row>
+    <row r="162" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A162" s="3" t="s">
         <v>11</v>
       </c>
@@ -3011,13 +3659,17 @@
         <v>50</v>
       </c>
       <c r="D162" s="3">
-        <v>70</v>
+        <v>19.444444599999997</v>
       </c>
       <c r="E162" s="3" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="163" spans="1:5" x14ac:dyDescent="0.3">
+        <v>32</v>
+      </c>
+      <c r="F162">
+        <f t="shared" si="2"/>
+        <v>5.4012346543209864</v>
+      </c>
+    </row>
+    <row r="163" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A163" s="3" t="s">
         <v>11</v>
       </c>
@@ -3028,13 +3680,17 @@
         <v>50</v>
       </c>
       <c r="D163" s="3">
-        <v>70</v>
+        <v>19.444444599999997</v>
       </c>
       <c r="E163" s="3" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="164" spans="1:5" ht="31.2" x14ac:dyDescent="0.3">
+        <v>32</v>
+      </c>
+      <c r="F163">
+        <f t="shared" si="2"/>
+        <v>5.4012346543209864</v>
+      </c>
+    </row>
+    <row r="164" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A164" s="3" t="s">
         <v>11</v>
       </c>
@@ -3045,13 +3701,17 @@
         <v>50</v>
       </c>
       <c r="D164" s="3">
-        <v>70</v>
+        <v>19.444444599999997</v>
       </c>
       <c r="E164" s="5" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="165" spans="1:5" x14ac:dyDescent="0.3">
+        <v>33</v>
+      </c>
+      <c r="F164">
+        <f t="shared" si="2"/>
+        <v>5.4012346543209864</v>
+      </c>
+    </row>
+    <row r="165" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A165" s="3" t="s">
         <v>11</v>
       </c>
@@ -3062,13 +3722,17 @@
         <v>50</v>
       </c>
       <c r="D165" s="3">
-        <v>70</v>
+        <v>19.444444599999997</v>
       </c>
       <c r="E165" s="3" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="166" spans="1:5" x14ac:dyDescent="0.3">
+        <v>32</v>
+      </c>
+      <c r="F165">
+        <f t="shared" si="2"/>
+        <v>5.4012346543209864</v>
+      </c>
+    </row>
+    <row r="166" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A166" s="3" t="s">
         <v>11</v>
       </c>
@@ -3079,13 +3743,17 @@
         <v>50</v>
       </c>
       <c r="D166" s="3">
-        <v>70</v>
+        <v>19.444444599999997</v>
       </c>
       <c r="E166" s="3" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="167" spans="1:5" x14ac:dyDescent="0.3">
+        <v>32</v>
+      </c>
+      <c r="F166">
+        <f t="shared" si="2"/>
+        <v>5.4012346543209864</v>
+      </c>
+    </row>
+    <row r="167" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A167" s="3" t="s">
         <v>11</v>
       </c>
@@ -3096,13 +3764,17 @@
         <v>50</v>
       </c>
       <c r="D167" s="3">
-        <v>70</v>
+        <v>19.444444599999997</v>
       </c>
       <c r="E167" s="3" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="168" spans="1:5" x14ac:dyDescent="0.3">
+        <v>32</v>
+      </c>
+      <c r="F167">
+        <f t="shared" si="2"/>
+        <v>5.4012346543209864</v>
+      </c>
+    </row>
+    <row r="168" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A168" s="3" t="s">
         <v>11</v>
       </c>
@@ -3113,13 +3785,17 @@
         <v>50</v>
       </c>
       <c r="D168" s="3">
-        <v>70</v>
+        <v>19.444444599999997</v>
       </c>
       <c r="E168" s="3" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="169" spans="1:5" x14ac:dyDescent="0.3">
+        <v>32</v>
+      </c>
+      <c r="F168">
+        <f t="shared" si="2"/>
+        <v>5.4012346543209864</v>
+      </c>
+    </row>
+    <row r="169" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A169" s="3" t="s">
         <v>11</v>
       </c>
@@ -3130,13 +3806,17 @@
         <v>50</v>
       </c>
       <c r="D169" s="3">
-        <v>70</v>
+        <v>19.444444599999997</v>
       </c>
       <c r="E169" s="3" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="170" spans="1:5" x14ac:dyDescent="0.3">
+        <v>32</v>
+      </c>
+      <c r="F169">
+        <f t="shared" si="2"/>
+        <v>5.4012346543209864</v>
+      </c>
+    </row>
+    <row r="170" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A170" s="3" t="s">
         <v>11</v>
       </c>
@@ -3147,13 +3827,17 @@
         <v>50</v>
       </c>
       <c r="D170" s="3">
-        <v>70</v>
+        <v>19.444444599999997</v>
       </c>
       <c r="E170" s="3" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="171" spans="1:5" x14ac:dyDescent="0.3">
+        <v>32</v>
+      </c>
+      <c r="F170">
+        <f t="shared" si="2"/>
+        <v>5.4012346543209864</v>
+      </c>
+    </row>
+    <row r="171" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A171" s="3" t="s">
         <v>11</v>
       </c>
@@ -3164,13 +3848,17 @@
         <v>50</v>
       </c>
       <c r="D171" s="3">
-        <v>70</v>
+        <v>19.444444599999997</v>
       </c>
       <c r="E171" s="3" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="172" spans="1:5" x14ac:dyDescent="0.3">
+        <v>32</v>
+      </c>
+      <c r="F171">
+        <f t="shared" si="2"/>
+        <v>5.4012346543209864</v>
+      </c>
+    </row>
+    <row r="172" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A172" s="3" t="s">
         <v>11</v>
       </c>
@@ -3181,13 +3869,17 @@
         <v>50</v>
       </c>
       <c r="D172" s="3">
-        <v>70</v>
+        <v>19.444444599999997</v>
       </c>
       <c r="E172" s="3" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="173" spans="1:5" ht="31.2" x14ac:dyDescent="0.3">
+        <v>32</v>
+      </c>
+      <c r="F172">
+        <f t="shared" si="2"/>
+        <v>5.4012346543209864</v>
+      </c>
+    </row>
+    <row r="173" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A173" s="3" t="s">
         <v>11</v>
       </c>
@@ -3198,15 +3890,19 @@
         <v>50</v>
       </c>
       <c r="D173" s="3">
-        <v>70</v>
+        <v>19.444444599999997</v>
       </c>
       <c r="E173" s="5" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="174" spans="1:5" x14ac:dyDescent="0.3">
+        <v>34</v>
+      </c>
+      <c r="F173">
+        <f t="shared" si="2"/>
+        <v>5.4012346543209864</v>
+      </c>
+    </row>
+    <row r="174" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A174" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B174" s="5">
         <v>151</v>
@@ -3215,13 +3911,17 @@
         <v>50</v>
       </c>
       <c r="D174" s="5">
-        <v>100</v>
+        <v>27.777777999999998</v>
       </c>
       <c r="E174" s="3" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="175" spans="1:5" x14ac:dyDescent="0.3">
+        <v>45</v>
+      </c>
+      <c r="F174">
+        <f t="shared" si="2"/>
+        <v>7.7160495061728387</v>
+      </c>
+    </row>
+    <row r="175" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A175" s="3" t="s">
         <v>12</v>
       </c>
@@ -3232,13 +3932,17 @@
         <v>50</v>
       </c>
       <c r="D175" s="3">
-        <v>60</v>
+        <v>16.666666799999998</v>
       </c>
       <c r="E175" s="5" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="176" spans="1:5" x14ac:dyDescent="0.3">
+        <v>35</v>
+      </c>
+      <c r="F175">
+        <f t="shared" si="2"/>
+        <v>4.6296297037037029</v>
+      </c>
+    </row>
+    <row r="176" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A176" s="3" t="s">
         <v>12</v>
       </c>
@@ -3249,10 +3953,14 @@
         <v>50</v>
       </c>
       <c r="D176" s="3">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="177" spans="1:4" x14ac:dyDescent="0.3">
+        <v>16.666666799999998</v>
+      </c>
+      <c r="F176">
+        <f t="shared" si="2"/>
+        <v>4.6296297037037029</v>
+      </c>
+    </row>
+    <row r="177" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A177" s="3" t="s">
         <v>12</v>
       </c>
@@ -3263,10 +3971,14 @@
         <v>50</v>
       </c>
       <c r="D177" s="3">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="178" spans="1:4" x14ac:dyDescent="0.3">
+        <v>16.666666799999998</v>
+      </c>
+      <c r="F177">
+        <f t="shared" si="2"/>
+        <v>4.6296297037037029</v>
+      </c>
+    </row>
+    <row r="178" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A178" s="3" t="s">
         <v>12</v>
       </c>
@@ -3277,100 +3989,104 @@
         <v>50</v>
       </c>
       <c r="D178" s="3">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="194" spans="4:4" x14ac:dyDescent="0.3">
+        <v>16.666666799999998</v>
+      </c>
+      <c r="F178">
+        <f t="shared" si="2"/>
+        <v>4.6296297037037029</v>
+      </c>
+    </row>
+    <row r="194" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D194" s="3"/>
     </row>
-    <row r="195" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="195" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D195" s="3"/>
     </row>
-    <row r="196" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="196" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D196" s="3"/>
     </row>
-    <row r="197" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="197" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D197" s="3"/>
     </row>
-    <row r="198" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="198" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D198" s="3"/>
     </row>
-    <row r="199" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="199" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D199" s="3"/>
     </row>
-    <row r="200" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="200" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D200" s="3"/>
     </row>
-    <row r="213" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="213" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A213" s="3"/>
       <c r="B213" s="4"/>
       <c r="C213" s="3"/>
       <c r="D213" s="3"/>
       <c r="E213" s="5"/>
     </row>
-    <row r="214" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="214" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A214" s="3"/>
       <c r="B214" s="3"/>
       <c r="C214" s="3"/>
       <c r="D214" s="3"/>
     </row>
-    <row r="215" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="215" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A215" s="3"/>
       <c r="B215" s="3"/>
       <c r="C215" s="3"/>
       <c r="D215" s="3"/>
       <c r="E215" s="5"/>
     </row>
-    <row r="216" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="216" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A216" s="3"/>
       <c r="B216" s="4"/>
       <c r="C216" s="3"/>
       <c r="D216" s="3"/>
     </row>
-    <row r="217" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="217" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A217" s="3"/>
       <c r="B217" s="3"/>
       <c r="C217" s="3"/>
       <c r="D217" s="3"/>
     </row>
-    <row r="218" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="218" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A218" s="3"/>
       <c r="B218" s="4"/>
       <c r="C218" s="3"/>
       <c r="D218" s="3"/>
     </row>
-    <row r="219" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="219" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A219" s="3"/>
       <c r="B219" s="4"/>
       <c r="C219" s="3"/>
       <c r="D219" s="3"/>
     </row>
-    <row r="220" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="220" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A220" s="3"/>
       <c r="B220" s="3"/>
       <c r="C220" s="3"/>
       <c r="D220" s="3"/>
     </row>
-    <row r="221" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="221" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A221" s="3"/>
       <c r="B221" s="3"/>
       <c r="C221" s="3"/>
       <c r="D221" s="3"/>
     </row>
-    <row r="222" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="222" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A222" s="3"/>
       <c r="B222" s="4"/>
       <c r="C222" s="3"/>
       <c r="D222" s="3"/>
     </row>
-    <row r="223" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="223" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A223" s="3"/>
       <c r="B223" s="3"/>
       <c r="C223" s="3"/>
       <c r="D223" s="3"/>
       <c r="E223" s="5"/>
     </row>
-    <row r="224" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="224" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A224" s="3"/>
       <c r="B224" s="3"/>
       <c r="C224" s="3"/>

</xml_diff>

<commit_message>
ctc block occupancies fixed
</commit_message>
<xml_diff>
--- a/modules/Green Line Info_.xlsx
+++ b/modules/Green Line Info_.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/52e6f4f7f86bcef2/Desktop/School/1140/1140/modules/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Desktop\School\1140\1140_iteration4\1140\modules\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="12" documentId="13_ncr:1_{8D4B131F-9DEC-48BC-972F-271BE62DE00D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B6296A60-270B-4979-9730-87888BC513B6}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1838E672-8A17-413B-A832-19215EC1231F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="220" yWindow="570" windowWidth="28800" windowHeight="15460" xr2:uid="{74BABC91-B30C-4EA1-9E18-CB507E7797A1}"/>
+    <workbookView xWindow="384" yWindow="384" windowWidth="17280" windowHeight="8964" xr2:uid="{74BABC91-B30C-4EA1-9E18-CB507E7797A1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -155,9 +155,6 @@
     <t>STATION; DORMONT</t>
   </si>
   <si>
-    <t>STATION;         MT LEBANON</t>
-  </si>
-  <si>
     <t>STATION; POPLAR</t>
   </si>
   <si>
@@ -183,6 +180,9 @@
   </si>
   <si>
     <t>Speed Limit (m/s)</t>
+  </si>
+  <si>
+    <t>STATION; MT LEBANON</t>
   </si>
 </sst>
 </file>
@@ -265,10 +265,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -568,18 +564,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E4104CD2-E043-4597-AF7D-F6AD80AEEABB}">
-  <dimension ref="A1:F224"/>
+  <dimension ref="A1:E224"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="5" max="5" width="37.54296875" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="37.5546875" style="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="46.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -590,19 +586,15 @@
         <v>2</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="F1" t="e">
-        <f>D1*0.27777778</f>
-        <v>#VALUE!</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B2" s="5">
         <v>151</v>
@@ -614,14 +606,10 @@
         <v>27.777777999999998</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="F2">
-        <f t="shared" ref="F2:F65" si="0">D2*0.27777778</f>
-        <v>7.7160495061728387</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>12</v>
       </c>
@@ -637,12 +625,8 @@
       <c r="E3" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="F3">
-        <f t="shared" si="0"/>
-        <v>4.6296297037037029</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>13</v>
       </c>
@@ -655,12 +639,8 @@
       <c r="D4" s="3">
         <v>19.444444599999997</v>
       </c>
-      <c r="F4">
-        <f t="shared" si="0"/>
-        <v>5.4012346543209864</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>13</v>
       </c>
@@ -673,12 +653,8 @@
       <c r="D5" s="3">
         <v>19.444444599999997</v>
       </c>
-      <c r="F5">
-        <f t="shared" si="0"/>
-        <v>5.4012346543209864</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
         <v>13</v>
       </c>
@@ -694,12 +670,8 @@
       <c r="E6" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="F6">
-        <f t="shared" si="0"/>
-        <v>5.4012346543209864</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
         <v>13</v>
       </c>
@@ -712,12 +684,8 @@
       <c r="D7" s="3">
         <v>19.444444599999997</v>
       </c>
-      <c r="F7">
-        <f t="shared" si="0"/>
-        <v>5.4012346543209864</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
         <v>13</v>
       </c>
@@ -730,12 +698,8 @@
       <c r="D8" s="3">
         <v>19.444444599999997</v>
       </c>
-      <c r="F8">
-        <f t="shared" si="0"/>
-        <v>5.4012346543209864</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
         <v>13</v>
       </c>
@@ -748,12 +712,8 @@
       <c r="D9" s="3">
         <v>19.444444599999997</v>
       </c>
-      <c r="F9">
-        <f t="shared" si="0"/>
-        <v>5.4012346543209864</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
         <v>14</v>
       </c>
@@ -766,12 +726,8 @@
       <c r="D10" s="3">
         <v>16.666666799999998</v>
       </c>
-      <c r="F10">
-        <f t="shared" si="0"/>
-        <v>4.6296297037037029</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
         <v>14</v>
       </c>
@@ -784,12 +740,8 @@
       <c r="D11" s="3">
         <v>16.666666799999998</v>
       </c>
-      <c r="F11">
-        <f t="shared" si="0"/>
-        <v>4.6296297037037029</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
         <v>14</v>
       </c>
@@ -802,12 +754,8 @@
       <c r="D12" s="3">
         <v>16.666666799999998</v>
       </c>
-      <c r="F12">
-        <f t="shared" si="0"/>
-        <v>4.6296297037037029</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
         <v>14</v>
       </c>
@@ -820,12 +768,8 @@
       <c r="D13" s="3">
         <v>16.666666799999998</v>
       </c>
-      <c r="F13">
-        <f t="shared" si="0"/>
-        <v>4.6296297037037029</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
         <v>14</v>
       </c>
@@ -841,12 +785,8 @@
       <c r="E14" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="F14">
-        <f t="shared" si="0"/>
-        <v>4.6296297037037029</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
         <v>15</v>
       </c>
@@ -859,12 +799,8 @@
       <c r="D15" s="3">
         <v>16.666666799999998</v>
       </c>
-      <c r="F15">
-        <f t="shared" si="0"/>
-        <v>4.6296297037037029</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="s">
         <v>15</v>
       </c>
@@ -877,12 +813,8 @@
       <c r="D16" s="3">
         <v>16.666666799999998</v>
       </c>
-      <c r="F16">
-        <f t="shared" si="0"/>
-        <v>4.6296297037037029</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" s="3" t="s">
         <v>15</v>
       </c>
@@ -898,12 +830,8 @@
       <c r="E17" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="F17">
-        <f t="shared" si="0"/>
-        <v>4.6296297037037029</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" s="3" t="s">
         <v>16</v>
       </c>
@@ -917,14 +845,10 @@
         <v>19.444444599999997</v>
       </c>
       <c r="E18" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="F18">
-        <f t="shared" si="0"/>
-        <v>5.4012346543209864</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" s="3" t="s">
         <v>16</v>
       </c>
@@ -937,12 +861,8 @@
       <c r="D19" s="3">
         <v>19.444444599999997</v>
       </c>
-      <c r="F19">
-        <f t="shared" si="0"/>
-        <v>5.4012346543209864</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" s="3" t="s">
         <v>16</v>
       </c>
@@ -955,12 +875,8 @@
       <c r="D20" s="3">
         <v>19.444444599999997</v>
       </c>
-      <c r="F20">
-        <f t="shared" si="0"/>
-        <v>5.4012346543209864</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" s="3" t="s">
         <v>16</v>
       </c>
@@ -973,12 +889,8 @@
       <c r="D21" s="3">
         <v>19.444444599999997</v>
       </c>
-      <c r="F21">
-        <f t="shared" si="0"/>
-        <v>5.4012346543209864</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" s="3" t="s">
         <v>16</v>
       </c>
@@ -991,12 +903,8 @@
       <c r="D22" s="3">
         <v>19.444444599999997</v>
       </c>
-      <c r="F22">
-        <f t="shared" si="0"/>
-        <v>5.4012346543209864</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" s="3" t="s">
         <v>16</v>
       </c>
@@ -1009,12 +917,8 @@
       <c r="D23" s="3">
         <v>19.444444599999997</v>
       </c>
-      <c r="F23">
-        <f t="shared" si="0"/>
-        <v>5.4012346543209864</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" s="3" t="s">
         <v>16</v>
       </c>
@@ -1027,12 +931,8 @@
       <c r="D24" s="3">
         <v>19.444444599999997</v>
       </c>
-      <c r="F24">
-        <f t="shared" si="0"/>
-        <v>5.4012346543209864</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" s="3" t="s">
         <v>16</v>
       </c>
@@ -1045,12 +945,8 @@
       <c r="D25" s="3">
         <v>19.444444599999997</v>
       </c>
-      <c r="F25">
-        <f t="shared" si="0"/>
-        <v>5.4012346543209864</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" s="3" t="s">
         <v>16</v>
       </c>
@@ -1063,12 +959,8 @@
       <c r="D26" s="3">
         <v>19.444444599999997</v>
       </c>
-      <c r="F26">
-        <f t="shared" si="0"/>
-        <v>5.4012346543209864</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" s="3" t="s">
         <v>17</v>
       </c>
@@ -1084,12 +976,8 @@
       <c r="E27" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="F27">
-        <f t="shared" si="0"/>
-        <v>4.2438272283950615</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" s="3" t="s">
         <v>17</v>
       </c>
@@ -1102,12 +990,8 @@
       <c r="D28" s="3">
         <v>15.277777899999998</v>
       </c>
-      <c r="F28">
-        <f t="shared" si="0"/>
-        <v>4.2438272283950615</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29" s="3" t="s">
         <v>17</v>
       </c>
@@ -1121,14 +1005,10 @@
         <v>15.277777899999998</v>
       </c>
       <c r="E29" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="F29">
-        <f t="shared" si="0"/>
-        <v>4.2438272283950615</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30" s="3" t="s">
         <v>18</v>
       </c>
@@ -1141,12 +1021,8 @@
       <c r="D30" s="3">
         <v>15.277777899999998</v>
       </c>
-      <c r="F30">
-        <f t="shared" si="0"/>
-        <v>4.2438272283950615</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.35">
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31" s="3" t="s">
         <v>18</v>
       </c>
@@ -1159,12 +1035,8 @@
       <c r="D31" s="3">
         <v>15.277777899999998</v>
       </c>
-      <c r="F31">
-        <f t="shared" si="0"/>
-        <v>4.2438272283950615</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.35">
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A32" s="3" t="s">
         <v>18</v>
       </c>
@@ -1177,12 +1049,8 @@
       <c r="D32" s="3">
         <v>15.277777899999998</v>
       </c>
-      <c r="F32">
-        <f t="shared" si="0"/>
-        <v>4.2438272283950615</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.35">
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A33" s="3" t="s">
         <v>18</v>
       </c>
@@ -1195,12 +1063,8 @@
       <c r="D33" s="3">
         <v>15.277777899999998</v>
       </c>
-      <c r="F33">
-        <f t="shared" si="0"/>
-        <v>4.2438272283950615</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.35">
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A34" s="3" t="s">
         <v>18</v>
       </c>
@@ -1213,12 +1077,8 @@
       <c r="D34" s="3">
         <v>15.277777899999998</v>
       </c>
-      <c r="F34">
-        <f t="shared" si="0"/>
-        <v>4.2438272283950615</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.35">
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A35" s="3" t="s">
         <v>18</v>
       </c>
@@ -1231,12 +1091,8 @@
       <c r="D35" s="3">
         <v>15.277777899999998</v>
       </c>
-      <c r="F35">
-        <f t="shared" si="0"/>
-        <v>4.2438272283950615</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.35">
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A36" s="3" t="s">
         <v>18</v>
       </c>
@@ -1249,12 +1105,8 @@
       <c r="D36" s="3">
         <v>15.277777899999998</v>
       </c>
-      <c r="F36">
-        <f t="shared" si="0"/>
-        <v>4.2438272283950615</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.35">
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A37" s="3" t="s">
         <v>18</v>
       </c>
@@ -1268,14 +1120,10 @@
         <v>15.277777899999998</v>
       </c>
       <c r="E37" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="F37">
-        <f t="shared" si="0"/>
-        <v>4.2438272283950615</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.35">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A38" s="3" t="s">
         <v>18</v>
       </c>
@@ -1288,12 +1136,8 @@
       <c r="D38" s="3">
         <v>15.277777899999998</v>
       </c>
-      <c r="F38">
-        <f t="shared" si="0"/>
-        <v>4.2438272283950615</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.35">
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A39" s="3" t="s">
         <v>19</v>
       </c>
@@ -1306,12 +1150,8 @@
       <c r="D39" s="3">
         <v>15.277777899999998</v>
       </c>
-      <c r="F39">
-        <f t="shared" si="0"/>
-        <v>4.2438272283950615</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.35">
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A40" s="3" t="s">
         <v>19</v>
       </c>
@@ -1324,12 +1164,8 @@
       <c r="D40" s="3">
         <v>15.277777899999998</v>
       </c>
-      <c r="F40">
-        <f t="shared" si="0"/>
-        <v>4.2438272283950615</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.35">
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A41" s="3" t="s">
         <v>19</v>
       </c>
@@ -1342,12 +1178,8 @@
       <c r="D41" s="3">
         <v>15.277777899999998</v>
       </c>
-      <c r="F41">
-        <f t="shared" si="0"/>
-        <v>4.2438272283950615</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.35">
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A42" s="3" t="s">
         <v>16</v>
       </c>
@@ -1360,12 +1192,8 @@
       <c r="D42" s="3">
         <v>19.444444599999997</v>
       </c>
-      <c r="F42">
-        <f t="shared" si="0"/>
-        <v>5.4012346543209864</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.35">
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A43" s="3" t="s">
         <v>16</v>
       </c>
@@ -1378,12 +1206,8 @@
       <c r="D43" s="3">
         <v>19.444444599999997</v>
       </c>
-      <c r="F43">
-        <f t="shared" si="0"/>
-        <v>5.4012346543209864</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.35">
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A44" s="3" t="s">
         <v>16</v>
       </c>
@@ -1396,12 +1220,8 @@
       <c r="D44" s="3">
         <v>19.444444599999997</v>
       </c>
-      <c r="F44">
-        <f t="shared" si="0"/>
-        <v>5.4012346543209864</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.35">
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A45" s="3" t="s">
         <v>16</v>
       </c>
@@ -1414,12 +1234,8 @@
       <c r="D45" s="3">
         <v>19.444444599999997</v>
       </c>
-      <c r="F45">
-        <f t="shared" si="0"/>
-        <v>5.4012346543209864</v>
-      </c>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.35">
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A46" s="3" t="s">
         <v>16</v>
       </c>
@@ -1432,12 +1248,8 @@
       <c r="D46" s="3">
         <v>19.444444599999997</v>
       </c>
-      <c r="F46">
-        <f t="shared" si="0"/>
-        <v>5.4012346543209864</v>
-      </c>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.35">
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A47" s="3" t="s">
         <v>16</v>
       </c>
@@ -1450,12 +1262,8 @@
       <c r="D47" s="3">
         <v>19.444444599999997</v>
       </c>
-      <c r="F47">
-        <f t="shared" si="0"/>
-        <v>5.4012346543209864</v>
-      </c>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.35">
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A48" s="3" t="s">
         <v>16</v>
       </c>
@@ -1468,12 +1276,8 @@
       <c r="D48" s="3">
         <v>19.444444599999997</v>
       </c>
-      <c r="F48">
-        <f t="shared" si="0"/>
-        <v>5.4012346543209864</v>
-      </c>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.35">
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A49" s="3" t="s">
         <v>16</v>
       </c>
@@ -1486,12 +1290,8 @@
       <c r="D49" s="3">
         <v>19.444444599999997</v>
       </c>
-      <c r="F49">
-        <f t="shared" si="0"/>
-        <v>5.4012346543209864</v>
-      </c>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.35">
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A50" s="3" t="s">
         <v>16</v>
       </c>
@@ -1504,12 +1304,8 @@
       <c r="D50" s="3">
         <v>19.444444599999997</v>
       </c>
-      <c r="F50">
-        <f t="shared" si="0"/>
-        <v>5.4012346543209864</v>
-      </c>
-    </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.35">
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A51" s="3" t="s">
         <v>20</v>
       </c>
@@ -1522,12 +1318,8 @@
       <c r="D51" s="3">
         <v>15.277777899999998</v>
       </c>
-      <c r="F51">
-        <f t="shared" si="0"/>
-        <v>4.2438272283950615</v>
-      </c>
-    </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.35">
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A52" s="3" t="s">
         <v>21</v>
       </c>
@@ -1540,12 +1332,8 @@
       <c r="D52" s="3">
         <v>16.666666799999998</v>
       </c>
-      <c r="F52">
-        <f t="shared" si="0"/>
-        <v>4.6296297037037029</v>
-      </c>
-    </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.35">
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A53" s="3" t="s">
         <v>21</v>
       </c>
@@ -1558,12 +1346,8 @@
       <c r="D53" s="3">
         <v>16.666666799999998</v>
       </c>
-      <c r="F53">
-        <f t="shared" si="0"/>
-        <v>4.6296297037037029</v>
-      </c>
-    </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.35">
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A54" s="3" t="s">
         <v>21</v>
       </c>
@@ -1576,12 +1360,8 @@
       <c r="D54" s="3">
         <v>16.666666799999998</v>
       </c>
-      <c r="F54">
-        <f t="shared" si="0"/>
-        <v>4.6296297037037029</v>
-      </c>
-    </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.35">
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A55" s="3" t="s">
         <v>22</v>
       </c>
@@ -1598,12 +1378,8 @@
         <f>E14</f>
         <v>STATION; DORMONT</v>
       </c>
-      <c r="F55">
-        <f t="shared" si="0"/>
-        <v>4.6296297037037029</v>
-      </c>
-    </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.35">
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A56" s="3" t="s">
         <v>22</v>
       </c>
@@ -1616,12 +1392,8 @@
       <c r="D56" s="3">
         <v>16.666666799999998</v>
       </c>
-      <c r="F56">
-        <f t="shared" si="0"/>
-        <v>4.6296297037037029</v>
-      </c>
-    </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.35">
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A57" s="3" t="s">
         <v>22</v>
       </c>
@@ -1634,12 +1406,8 @@
       <c r="D57" s="3">
         <v>16.666666799999998</v>
       </c>
-      <c r="F57">
-        <f t="shared" si="0"/>
-        <v>4.6296297037037029</v>
-      </c>
-    </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.35">
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A58" s="3" t="s">
         <v>22</v>
       </c>
@@ -1652,12 +1420,8 @@
       <c r="D58" s="3">
         <v>16.666666799999998</v>
       </c>
-      <c r="F58">
-        <f t="shared" si="0"/>
-        <v>4.6296297037037029</v>
-      </c>
-    </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.35">
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A59" s="3" t="s">
         <v>22</v>
       </c>
@@ -1670,12 +1434,8 @@
       <c r="D59" s="3">
         <v>16.666666799999998</v>
       </c>
-      <c r="F59">
-        <f t="shared" si="0"/>
-        <v>4.6296297037037029</v>
-      </c>
-    </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.35">
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A60" s="3" t="s">
         <v>23</v>
       </c>
@@ -1688,12 +1448,8 @@
       <c r="D60" s="3">
         <v>19.444444599999997</v>
       </c>
-      <c r="F60">
-        <f t="shared" si="0"/>
-        <v>5.4012346543209864</v>
-      </c>
-    </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.35">
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A61" s="3" t="s">
         <v>23</v>
       </c>
@@ -1706,12 +1462,8 @@
       <c r="D61" s="3">
         <v>19.444444599999997</v>
       </c>
-      <c r="F61">
-        <f t="shared" si="0"/>
-        <v>5.4012346543209864</v>
-      </c>
-    </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.35">
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A62" s="3" t="s">
         <v>23</v>
       </c>
@@ -1724,12 +1476,8 @@
       <c r="D62" s="3">
         <v>19.444444599999997</v>
       </c>
-      <c r="F62">
-        <f t="shared" si="0"/>
-        <v>5.4012346543209864</v>
-      </c>
-    </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.35">
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A63" s="3" t="s">
         <v>23</v>
       </c>
@@ -1742,12 +1490,8 @@
       <c r="D63" s="3">
         <v>19.444444599999997</v>
       </c>
-      <c r="F63">
-        <f t="shared" si="0"/>
-        <v>5.4012346543209864</v>
-      </c>
-    </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.35">
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A64" s="3" t="s">
         <v>23</v>
       </c>
@@ -1764,12 +1508,8 @@
         <f>E6</f>
         <v>STATION; GLENBURY</v>
       </c>
-      <c r="F64">
-        <f t="shared" si="0"/>
-        <v>5.4012346543209864</v>
-      </c>
-    </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.35">
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A65" s="3" t="s">
         <v>23</v>
       </c>
@@ -1782,12 +1522,8 @@
       <c r="D65" s="3">
         <v>19.444444599999997</v>
       </c>
-      <c r="F65">
-        <f t="shared" si="0"/>
-        <v>5.4012346543209864</v>
-      </c>
-    </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.35">
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A66" s="3" t="s">
         <v>23</v>
       </c>
@@ -1800,12 +1536,8 @@
       <c r="D66" s="3">
         <v>19.444444599999997</v>
       </c>
-      <c r="F66">
-        <f t="shared" ref="F66:F129" si="1">D66*0.27777778</f>
-        <v>5.4012346543209864</v>
-      </c>
-    </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.35">
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A67" s="3" t="s">
         <v>24</v>
       </c>
@@ -1818,12 +1550,8 @@
       <c r="D67" s="3">
         <v>16.666666799999998</v>
       </c>
-      <c r="F67">
-        <f t="shared" si="1"/>
-        <v>4.6296297037037029</v>
-      </c>
-    </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.35">
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A68" s="3" t="s">
         <v>24</v>
       </c>
@@ -1836,12 +1564,8 @@
       <c r="D68" s="3">
         <v>16.666666799999998</v>
       </c>
-      <c r="F68">
-        <f t="shared" si="1"/>
-        <v>4.6296297037037029</v>
-      </c>
-    </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.35">
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A69" s="3" t="s">
         <v>24</v>
       </c>
@@ -1854,12 +1578,8 @@
       <c r="D69" s="3">
         <v>16.666666799999998</v>
       </c>
-      <c r="F69">
-        <f t="shared" si="1"/>
-        <v>4.6296297037037029</v>
-      </c>
-    </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.35">
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A70" s="3" t="s">
         <v>24</v>
       </c>
@@ -1872,12 +1592,8 @@
       <c r="D70" s="3">
         <v>16.666666799999998</v>
       </c>
-      <c r="F70">
-        <f t="shared" si="1"/>
-        <v>4.6296297037037029</v>
-      </c>
-    </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.35">
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A71" s="3" t="s">
         <v>24</v>
       </c>
@@ -1890,12 +1606,8 @@
       <c r="D71" s="3">
         <v>16.666666799999998</v>
       </c>
-      <c r="F71">
-        <f t="shared" si="1"/>
-        <v>4.6296297037037029</v>
-      </c>
-    </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.35">
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A72" s="3" t="s">
         <v>25</v>
       </c>
@@ -1911,12 +1623,8 @@
       <c r="E72" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="F72">
-        <f t="shared" si="1"/>
-        <v>5.4012346543209864</v>
-      </c>
-    </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.35">
+    </row>
+    <row r="73" spans="1:5" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A73" s="3" t="s">
         <v>25</v>
       </c>
@@ -1933,12 +1641,8 @@
         <f>E173</f>
         <v>STATION; OVERBROOK; UNDERGROUND</v>
       </c>
-      <c r="F73">
-        <f t="shared" si="1"/>
-        <v>5.4012346543209864</v>
-      </c>
-    </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.35">
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A74" s="3" t="s">
         <v>25</v>
       </c>
@@ -1954,12 +1658,8 @@
       <c r="E74" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="F74">
-        <f t="shared" si="1"/>
-        <v>5.4012346543209864</v>
-      </c>
-    </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.35">
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A75" s="3" t="s">
         <v>25</v>
       </c>
@@ -1975,12 +1675,8 @@
       <c r="E75" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="F75">
-        <f t="shared" si="1"/>
-        <v>5.4012346543209864</v>
-      </c>
-    </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.35">
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A76" s="3" t="s">
         <v>25</v>
       </c>
@@ -1996,12 +1692,8 @@
       <c r="E76" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="F76">
-        <f t="shared" si="1"/>
-        <v>5.4012346543209864</v>
-      </c>
-    </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.35">
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A77" s="3" t="s">
         <v>25</v>
       </c>
@@ -2017,12 +1709,8 @@
       <c r="E77" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="F77">
-        <f t="shared" si="1"/>
-        <v>5.4012346543209864</v>
-      </c>
-    </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.35">
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A78" s="3" t="s">
         <v>25</v>
       </c>
@@ -2038,12 +1726,8 @@
       <c r="E78" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="F78">
-        <f t="shared" si="1"/>
-        <v>5.4012346543209864</v>
-      </c>
-    </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.35">
+    </row>
+    <row r="79" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A79" s="3" t="s">
         <v>25</v>
       </c>
@@ -2059,12 +1743,8 @@
       <c r="E79" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="F79">
-        <f t="shared" si="1"/>
-        <v>5.4012346543209864</v>
-      </c>
-    </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.35">
+    </row>
+    <row r="80" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A80" s="3" t="s">
         <v>25</v>
       </c>
@@ -2080,12 +1760,8 @@
       <c r="E80" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="F80">
-        <f t="shared" si="1"/>
-        <v>5.4012346543209864</v>
-      </c>
-    </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.35">
+    </row>
+    <row r="81" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A81" s="3" t="s">
         <v>25</v>
       </c>
@@ -2101,12 +1777,8 @@
       <c r="E81" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="F81">
-        <f t="shared" si="1"/>
-        <v>5.4012346543209864</v>
-      </c>
-    </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.35">
+    </row>
+    <row r="82" spans="1:5" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A82" s="3" t="s">
         <v>25</v>
       </c>
@@ -2123,12 +1795,8 @@
         <f>E164</f>
         <v>STATION; INGLEWOOD; UNDERGROUND</v>
       </c>
-      <c r="F82">
-        <f t="shared" si="1"/>
-        <v>5.4012346543209864</v>
-      </c>
-    </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.35">
+    </row>
+    <row r="83" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A83" s="3" t="s">
         <v>25</v>
       </c>
@@ -2144,12 +1812,8 @@
       <c r="E83" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="F83">
-        <f t="shared" si="1"/>
-        <v>5.4012346543209864</v>
-      </c>
-    </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.35">
+    </row>
+    <row r="84" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A84" s="3" t="s">
         <v>25</v>
       </c>
@@ -2165,12 +1829,8 @@
       <c r="E84" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="F84">
-        <f t="shared" si="1"/>
-        <v>5.4012346543209864</v>
-      </c>
-    </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.35">
+    </row>
+    <row r="85" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A85" s="3" t="s">
         <v>25</v>
       </c>
@@ -2186,12 +1846,8 @@
       <c r="E85" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="F85">
-        <f t="shared" si="1"/>
-        <v>5.4012346543209864</v>
-      </c>
-    </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.35">
+    </row>
+    <row r="86" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A86" s="3" t="s">
         <v>25</v>
       </c>
@@ -2207,12 +1863,8 @@
       <c r="E86" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="F86">
-        <f t="shared" si="1"/>
-        <v>5.4012346543209864</v>
-      </c>
-    </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.35">
+    </row>
+    <row r="87" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A87" s="3" t="s">
         <v>25</v>
       </c>
@@ -2228,12 +1880,8 @@
       <c r="E87" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="F87">
-        <f t="shared" si="1"/>
-        <v>5.4012346543209864</v>
-      </c>
-    </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.35">
+    </row>
+    <row r="88" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A88" s="3" t="s">
         <v>25</v>
       </c>
@@ -2249,12 +1897,8 @@
       <c r="E88" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="F88">
-        <f t="shared" si="1"/>
-        <v>5.4012346543209864</v>
-      </c>
-    </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.35">
+    </row>
+    <row r="89" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A89" s="3" t="s">
         <v>25</v>
       </c>
@@ -2270,12 +1914,8 @@
       <c r="E89" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="F89">
-        <f t="shared" si="1"/>
-        <v>5.4012346543209864</v>
-      </c>
-    </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.35">
+    </row>
+    <row r="90" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A90" s="3" t="s">
         <v>25</v>
       </c>
@@ -2291,12 +1931,8 @@
       <c r="E90" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="F90">
-        <f t="shared" si="1"/>
-        <v>5.4012346543209864</v>
-      </c>
-    </row>
-    <row r="91" spans="1:6" x14ac:dyDescent="0.35">
+    </row>
+    <row r="91" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A91" s="3" t="s">
         <v>25</v>
       </c>
@@ -2313,12 +1949,8 @@
         <f>E155</f>
         <v>STATION; CENTRAL; UNDERGROUND</v>
       </c>
-      <c r="F91">
-        <f t="shared" si="1"/>
-        <v>5.4012346543209864</v>
-      </c>
-    </row>
-    <row r="92" spans="1:6" x14ac:dyDescent="0.35">
+    </row>
+    <row r="92" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A92" s="3" t="s">
         <v>25</v>
       </c>
@@ -2334,12 +1966,8 @@
       <c r="E92" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="F92">
-        <f t="shared" si="1"/>
-        <v>5.4012346543209864</v>
-      </c>
-    </row>
-    <row r="93" spans="1:6" x14ac:dyDescent="0.35">
+    </row>
+    <row r="93" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A93" s="3" t="s">
         <v>25</v>
       </c>
@@ -2355,14 +1983,10 @@
       <c r="E93" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="F93">
-        <f t="shared" si="1"/>
-        <v>5.4012346543209864</v>
-      </c>
-    </row>
-    <row r="94" spans="1:6" x14ac:dyDescent="0.35">
+    </row>
+    <row r="94" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A94" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B94" s="3">
         <v>144</v>
@@ -2374,14 +1998,10 @@
         <v>19.444444599999997</v>
       </c>
       <c r="E94" s="5"/>
-      <c r="F94">
-        <f t="shared" si="1"/>
-        <v>5.4012346543209864</v>
-      </c>
-    </row>
-    <row r="95" spans="1:6" x14ac:dyDescent="0.35">
+    </row>
+    <row r="95" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A95" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B95" s="3">
         <v>145</v>
@@ -2393,14 +2013,10 @@
         <v>19.444444599999997</v>
       </c>
       <c r="E95" s="5"/>
-      <c r="F95">
-        <f t="shared" si="1"/>
-        <v>5.4012346543209864</v>
-      </c>
-    </row>
-    <row r="96" spans="1:6" x14ac:dyDescent="0.35">
+    </row>
+    <row r="96" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A96" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B96" s="3">
         <v>146</v>
@@ -2412,14 +2028,10 @@
         <v>19.444444599999997</v>
       </c>
       <c r="E96" s="5"/>
-      <c r="F96">
-        <f t="shared" si="1"/>
-        <v>5.4012346543209864</v>
-      </c>
-    </row>
-    <row r="97" spans="1:6" x14ac:dyDescent="0.35">
+    </row>
+    <row r="97" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A97" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B97" s="3">
         <v>147</v>
@@ -2431,14 +2043,10 @@
         <v>19.444444599999997</v>
       </c>
       <c r="E97" s="5"/>
-      <c r="F97">
-        <f t="shared" si="1"/>
-        <v>5.4012346543209864</v>
-      </c>
-    </row>
-    <row r="98" spans="1:6" x14ac:dyDescent="0.35">
+    </row>
+    <row r="98" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A98" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B98" s="3">
         <v>148</v>
@@ -2450,14 +2058,10 @@
         <v>19.444444599999997</v>
       </c>
       <c r="E98" s="5"/>
-      <c r="F98">
-        <f t="shared" si="1"/>
-        <v>5.4012346543209864</v>
-      </c>
-    </row>
-    <row r="99" spans="1:6" x14ac:dyDescent="0.35">
+    </row>
+    <row r="99" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A99" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B99" s="3">
         <v>149</v>
@@ -2469,14 +2073,10 @@
         <v>19.444444599999997</v>
       </c>
       <c r="E99" s="5"/>
-      <c r="F99">
-        <f t="shared" si="1"/>
-        <v>5.4012346543209864</v>
-      </c>
-    </row>
-    <row r="100" spans="1:6" x14ac:dyDescent="0.35">
+    </row>
+    <row r="100" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A100" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B100" s="3">
         <v>150</v>
@@ -2488,12 +2088,8 @@
         <v>19.444444599999997</v>
       </c>
       <c r="E100" s="5"/>
-      <c r="F100">
-        <f t="shared" si="1"/>
-        <v>5.4012346543209864</v>
-      </c>
-    </row>
-    <row r="101" spans="1:6" x14ac:dyDescent="0.35">
+    </row>
+    <row r="101" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A101" s="3" t="s">
         <v>8</v>
       </c>
@@ -2507,12 +2103,8 @@
         <v>19.444444599999997</v>
       </c>
       <c r="E101" s="5"/>
-      <c r="F101">
-        <f t="shared" si="1"/>
-        <v>5.4012346543209864</v>
-      </c>
-    </row>
-    <row r="102" spans="1:6" x14ac:dyDescent="0.35">
+    </row>
+    <row r="102" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A102" s="3" t="s">
         <v>8</v>
       </c>
@@ -2526,12 +2118,8 @@
         <v>19.444444599999997</v>
       </c>
       <c r="E102" s="5"/>
-      <c r="F102">
-        <f t="shared" si="1"/>
-        <v>5.4012346543209864</v>
-      </c>
-    </row>
-    <row r="103" spans="1:6" x14ac:dyDescent="0.35">
+    </row>
+    <row r="103" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A103" s="3" t="s">
         <v>8</v>
       </c>
@@ -2545,12 +2133,8 @@
         <v>19.444444599999997</v>
       </c>
       <c r="E103" s="5"/>
-      <c r="F103">
-        <f t="shared" si="1"/>
-        <v>5.4012346543209864</v>
-      </c>
-    </row>
-    <row r="104" spans="1:6" x14ac:dyDescent="0.35">
+    </row>
+    <row r="104" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A104" s="3" t="s">
         <v>8</v>
       </c>
@@ -2563,12 +2147,8 @@
       <c r="D104" s="3">
         <v>19.444444599999997</v>
       </c>
-      <c r="F104">
-        <f t="shared" si="1"/>
-        <v>5.4012346543209864</v>
-      </c>
-    </row>
-    <row r="105" spans="1:6" x14ac:dyDescent="0.35">
+    </row>
+    <row r="105" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A105" s="3" t="s">
         <v>8</v>
       </c>
@@ -2581,12 +2161,8 @@
       <c r="D105" s="3">
         <v>19.444444599999997</v>
       </c>
-      <c r="F105">
-        <f t="shared" si="1"/>
-        <v>5.4012346543209864</v>
-      </c>
-    </row>
-    <row r="106" spans="1:6" x14ac:dyDescent="0.35">
+    </row>
+    <row r="106" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A106" s="3" t="s">
         <v>8</v>
       </c>
@@ -2599,12 +2175,8 @@
       <c r="D106" s="3">
         <v>19.444444599999997</v>
       </c>
-      <c r="F106">
-        <f t="shared" si="1"/>
-        <v>5.4012346543209864</v>
-      </c>
-    </row>
-    <row r="107" spans="1:6" x14ac:dyDescent="0.35">
+    </row>
+    <row r="107" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A107" s="3" t="s">
         <v>8</v>
       </c>
@@ -2620,12 +2192,8 @@
       <c r="E107" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="F107">
-        <f t="shared" si="1"/>
-        <v>5.4012346543209864</v>
-      </c>
-    </row>
-    <row r="108" spans="1:6" x14ac:dyDescent="0.35">
+    </row>
+    <row r="108" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A108" s="3" t="s">
         <v>8</v>
       </c>
@@ -2638,12 +2206,8 @@
       <c r="D108" s="3">
         <v>19.444444599999997</v>
       </c>
-      <c r="F108">
-        <f t="shared" si="1"/>
-        <v>5.4012346543209864</v>
-      </c>
-    </row>
-    <row r="109" spans="1:6" x14ac:dyDescent="0.35">
+    </row>
+    <row r="109" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A109" s="3" t="s">
         <v>7</v>
       </c>
@@ -2656,12 +2220,8 @@
       <c r="D109" s="3">
         <v>16.666666799999998</v>
       </c>
-      <c r="F109">
-        <f t="shared" si="1"/>
-        <v>4.6296297037037029</v>
-      </c>
-    </row>
-    <row r="110" spans="1:6" x14ac:dyDescent="0.35">
+    </row>
+    <row r="110" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A110" s="3" t="s">
         <v>7</v>
       </c>
@@ -2674,12 +2234,8 @@
       <c r="D110" s="3">
         <v>16.666666799999998</v>
       </c>
-      <c r="F110">
-        <f t="shared" si="1"/>
-        <v>4.6296297037037029</v>
-      </c>
-    </row>
-    <row r="111" spans="1:6" x14ac:dyDescent="0.35">
+    </row>
+    <row r="111" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A111" s="3" t="s">
         <v>7</v>
       </c>
@@ -2692,12 +2248,8 @@
       <c r="D111" s="3">
         <v>16.666666799999998</v>
       </c>
-      <c r="F111">
-        <f t="shared" si="1"/>
-        <v>4.6296297037037029</v>
-      </c>
-    </row>
-    <row r="112" spans="1:6" x14ac:dyDescent="0.35">
+    </row>
+    <row r="112" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A112" s="3" t="s">
         <v>7</v>
       </c>
@@ -2710,12 +2262,8 @@
       <c r="D112" s="3">
         <v>16.666666799999998</v>
       </c>
-      <c r="F112">
-        <f t="shared" si="1"/>
-        <v>4.6296297037037029</v>
-      </c>
-    </row>
-    <row r="113" spans="1:6" x14ac:dyDescent="0.35">
+    </row>
+    <row r="113" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A113" s="3" t="s">
         <v>6</v>
       </c>
@@ -2729,14 +2277,10 @@
         <v>19.444444599999997</v>
       </c>
       <c r="E113" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="F113">
-        <f t="shared" si="1"/>
-        <v>5.4012346543209864</v>
-      </c>
-    </row>
-    <row r="114" spans="1:6" x14ac:dyDescent="0.35">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="114" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A114" s="3" t="s">
         <v>6</v>
       </c>
@@ -2749,12 +2293,8 @@
       <c r="D114" s="3">
         <v>19.444444599999997</v>
       </c>
-      <c r="F114">
-        <f t="shared" si="1"/>
-        <v>5.4012346543209864</v>
-      </c>
-    </row>
-    <row r="115" spans="1:6" x14ac:dyDescent="0.35">
+    </row>
+    <row r="115" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A115" s="3" t="s">
         <v>6</v>
       </c>
@@ -2767,12 +2307,8 @@
       <c r="D115" s="3">
         <v>19.444444599999997</v>
       </c>
-      <c r="F115">
-        <f t="shared" si="1"/>
-        <v>5.4012346543209864</v>
-      </c>
-    </row>
-    <row r="116" spans="1:6" x14ac:dyDescent="0.35">
+    </row>
+    <row r="116" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A116" s="3" t="s">
         <v>6</v>
       </c>
@@ -2785,12 +2321,8 @@
       <c r="D116" s="3">
         <v>19.444444599999997</v>
       </c>
-      <c r="F116">
-        <f t="shared" si="1"/>
-        <v>5.4012346543209864</v>
-      </c>
-    </row>
-    <row r="117" spans="1:6" x14ac:dyDescent="0.35">
+    </row>
+    <row r="117" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A117" s="3" t="s">
         <v>5</v>
       </c>
@@ -2806,12 +2338,8 @@
       <c r="E117" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="F117">
-        <f t="shared" si="1"/>
-        <v>4.2438272283950615</v>
-      </c>
-    </row>
-    <row r="118" spans="1:6" x14ac:dyDescent="0.35">
+    </row>
+    <row r="118" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A118" s="3" t="s">
         <v>5</v>
       </c>
@@ -2824,12 +2352,8 @@
       <c r="D118" s="3">
         <v>15.277777899999998</v>
       </c>
-      <c r="F118">
-        <f t="shared" si="1"/>
-        <v>4.2438272283950615</v>
-      </c>
-    </row>
-    <row r="119" spans="1:6" x14ac:dyDescent="0.35">
+    </row>
+    <row r="119" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A119" s="3" t="s">
         <v>5</v>
       </c>
@@ -2842,12 +2366,8 @@
       <c r="D119" s="3">
         <v>15.277777899999998</v>
       </c>
-      <c r="F119">
-        <f t="shared" si="1"/>
-        <v>4.2438272283950615</v>
-      </c>
-    </row>
-    <row r="120" spans="1:6" x14ac:dyDescent="0.35">
+    </row>
+    <row r="120" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A120" s="3" t="s">
         <v>5</v>
       </c>
@@ -2863,12 +2383,8 @@
       <c r="E120" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="F120">
-        <f t="shared" si="1"/>
-        <v>4.2438272283950615</v>
-      </c>
-    </row>
-    <row r="121" spans="1:6" x14ac:dyDescent="0.35">
+    </row>
+    <row r="121" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A121" s="3" t="s">
         <v>5</v>
       </c>
@@ -2881,12 +2397,8 @@
       <c r="D121" s="3">
         <v>15.277777899999998</v>
       </c>
-      <c r="F121">
-        <f t="shared" si="1"/>
-        <v>4.2438272283950615</v>
-      </c>
-    </row>
-    <row r="122" spans="1:6" x14ac:dyDescent="0.35">
+    </row>
+    <row r="122" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A122" s="3" t="s">
         <v>5</v>
       </c>
@@ -2899,12 +2411,8 @@
       <c r="D122" s="3">
         <v>15.277777899999998</v>
       </c>
-      <c r="F122">
-        <f t="shared" si="1"/>
-        <v>4.2438272283950615</v>
-      </c>
-    </row>
-    <row r="123" spans="1:6" x14ac:dyDescent="0.35">
+    </row>
+    <row r="123" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A123" s="3" t="s">
         <v>4</v>
       </c>
@@ -2917,12 +2425,8 @@
       <c r="D123" s="3">
         <v>15.277777899999998</v>
       </c>
-      <c r="F123">
-        <f t="shared" si="1"/>
-        <v>4.2438272283950615</v>
-      </c>
-    </row>
-    <row r="124" spans="1:6" x14ac:dyDescent="0.35">
+    </row>
+    <row r="124" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A124" s="3" t="s">
         <v>4</v>
       </c>
@@ -2935,12 +2439,8 @@
       <c r="D124" s="3">
         <v>15.277777899999998</v>
       </c>
-      <c r="F124">
-        <f t="shared" si="1"/>
-        <v>4.2438272283950615</v>
-      </c>
-    </row>
-    <row r="125" spans="1:6" x14ac:dyDescent="0.35">
+    </row>
+    <row r="125" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A125" s="3" t="s">
         <v>4</v>
       </c>
@@ -2953,12 +2453,8 @@
       <c r="D125" s="3">
         <v>15.277777899999998</v>
       </c>
-      <c r="F125">
-        <f t="shared" si="1"/>
-        <v>4.2438272283950615</v>
-      </c>
-    </row>
-    <row r="126" spans="1:6" x14ac:dyDescent="0.35">
+    </row>
+    <row r="126" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A126" s="3" t="s">
         <v>3</v>
       </c>
@@ -2971,12 +2467,8 @@
       <c r="D126" s="3">
         <v>15.277777899999998</v>
       </c>
-      <c r="F126">
-        <f t="shared" si="1"/>
-        <v>4.2438272283950615</v>
-      </c>
-    </row>
-    <row r="127" spans="1:6" x14ac:dyDescent="0.35">
+    </row>
+    <row r="127" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A127" s="3" t="s">
         <v>3</v>
       </c>
@@ -2992,12 +2484,8 @@
       <c r="E127" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="F127">
-        <f t="shared" si="1"/>
-        <v>4.2438272283950615</v>
-      </c>
-    </row>
-    <row r="128" spans="1:6" x14ac:dyDescent="0.35">
+    </row>
+    <row r="128" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A128" s="3" t="s">
         <v>3</v>
       </c>
@@ -3010,12 +2498,8 @@
       <c r="D128" s="3">
         <v>15.277777899999998</v>
       </c>
-      <c r="F128">
-        <f t="shared" si="1"/>
-        <v>4.2438272283950615</v>
-      </c>
-    </row>
-    <row r="129" spans="1:6" x14ac:dyDescent="0.35">
+    </row>
+    <row r="129" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A129" s="3" t="s">
         <v>6</v>
       </c>
@@ -3028,12 +2512,8 @@
       <c r="D129" s="3">
         <v>19.444444599999997</v>
       </c>
-      <c r="F129">
-        <f t="shared" si="1"/>
-        <v>5.4012346543209864</v>
-      </c>
-    </row>
-    <row r="130" spans="1:6" x14ac:dyDescent="0.35">
+    </row>
+    <row r="130" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A130" s="3" t="s">
         <v>6</v>
       </c>
@@ -3046,12 +2526,8 @@
       <c r="D130" s="3">
         <v>19.444444599999997</v>
       </c>
-      <c r="F130">
-        <f t="shared" ref="F130:F178" si="2">D130*0.27777778</f>
-        <v>5.4012346543209864</v>
-      </c>
-    </row>
-    <row r="131" spans="1:6" x14ac:dyDescent="0.35">
+    </row>
+    <row r="131" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A131" s="3" t="s">
         <v>6</v>
       </c>
@@ -3064,12 +2540,8 @@
       <c r="D131" s="3">
         <v>19.444444599999997</v>
       </c>
-      <c r="F131">
-        <f t="shared" si="2"/>
-        <v>5.4012346543209864</v>
-      </c>
-    </row>
-    <row r="132" spans="1:6" x14ac:dyDescent="0.35">
+    </row>
+    <row r="132" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A132" s="3" t="s">
         <v>6</v>
       </c>
@@ -3083,14 +2555,10 @@
         <v>19.444444599999997</v>
       </c>
       <c r="E132" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="F132">
-        <f t="shared" si="2"/>
-        <v>5.4012346543209864</v>
-      </c>
-    </row>
-    <row r="133" spans="1:6" x14ac:dyDescent="0.35">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="133" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A133" s="3" t="s">
         <v>7</v>
       </c>
@@ -3103,12 +2571,8 @@
       <c r="D133" s="3">
         <v>16.666666799999998</v>
       </c>
-      <c r="F133">
-        <f t="shared" si="2"/>
-        <v>4.6296297037037029</v>
-      </c>
-    </row>
-    <row r="134" spans="1:6" x14ac:dyDescent="0.35">
+    </row>
+    <row r="134" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A134" s="3" t="s">
         <v>7</v>
       </c>
@@ -3121,12 +2585,8 @@
       <c r="D134" s="3">
         <v>16.666666799999998</v>
       </c>
-      <c r="F134">
-        <f t="shared" si="2"/>
-        <v>4.6296297037037029</v>
-      </c>
-    </row>
-    <row r="135" spans="1:6" x14ac:dyDescent="0.35">
+    </row>
+    <row r="135" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A135" s="3" t="s">
         <v>7</v>
       </c>
@@ -3139,12 +2599,8 @@
       <c r="D135" s="3">
         <v>16.666666799999998</v>
       </c>
-      <c r="F135">
-        <f t="shared" si="2"/>
-        <v>4.6296297037037029</v>
-      </c>
-    </row>
-    <row r="136" spans="1:6" x14ac:dyDescent="0.35">
+    </row>
+    <row r="136" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A136" s="3" t="s">
         <v>7</v>
       </c>
@@ -3157,12 +2613,8 @@
       <c r="D136" s="3">
         <v>16.666666799999998</v>
       </c>
-      <c r="F136">
-        <f t="shared" si="2"/>
-        <v>4.6296297037037029</v>
-      </c>
-    </row>
-    <row r="137" spans="1:6" x14ac:dyDescent="0.35">
+    </row>
+    <row r="137" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A137" s="3" t="s">
         <v>8</v>
       </c>
@@ -3175,12 +2627,8 @@
       <c r="D137" s="3">
         <v>19.444444599999997</v>
       </c>
-      <c r="F137">
-        <f t="shared" si="2"/>
-        <v>5.4012346543209864</v>
-      </c>
-    </row>
-    <row r="138" spans="1:6" x14ac:dyDescent="0.35">
+    </row>
+    <row r="138" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A138" s="3" t="s">
         <v>8</v>
       </c>
@@ -3193,12 +2641,8 @@
       <c r="D138" s="3">
         <v>19.444444599999997</v>
       </c>
-      <c r="F138">
-        <f t="shared" si="2"/>
-        <v>5.4012346543209864</v>
-      </c>
-    </row>
-    <row r="139" spans="1:6" x14ac:dyDescent="0.35">
+    </row>
+    <row r="139" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A139" s="3" t="s">
         <v>8</v>
       </c>
@@ -3211,12 +2655,8 @@
       <c r="D139" s="3">
         <v>19.444444599999997</v>
       </c>
-      <c r="F139">
-        <f t="shared" si="2"/>
-        <v>5.4012346543209864</v>
-      </c>
-    </row>
-    <row r="140" spans="1:6" x14ac:dyDescent="0.35">
+    </row>
+    <row r="140" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A140" s="3" t="s">
         <v>8</v>
       </c>
@@ -3229,12 +2669,8 @@
       <c r="D140" s="3">
         <v>19.444444599999997</v>
       </c>
-      <c r="F140">
-        <f t="shared" si="2"/>
-        <v>5.4012346543209864</v>
-      </c>
-    </row>
-    <row r="141" spans="1:6" x14ac:dyDescent="0.35">
+    </row>
+    <row r="141" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A141" s="3" t="s">
         <v>8</v>
       </c>
@@ -3247,12 +2683,8 @@
       <c r="D141" s="3">
         <v>19.444444599999997</v>
       </c>
-      <c r="F141">
-        <f t="shared" si="2"/>
-        <v>5.4012346543209864</v>
-      </c>
-    </row>
-    <row r="142" spans="1:6" x14ac:dyDescent="0.35">
+    </row>
+    <row r="142" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A142" s="3" t="s">
         <v>8</v>
       </c>
@@ -3265,12 +2697,8 @@
       <c r="D142" s="3">
         <v>19.444444599999997</v>
       </c>
-      <c r="F142">
-        <f t="shared" si="2"/>
-        <v>5.4012346543209864</v>
-      </c>
-    </row>
-    <row r="143" spans="1:6" x14ac:dyDescent="0.35">
+    </row>
+    <row r="143" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A143" s="3" t="s">
         <v>8</v>
       </c>
@@ -3283,12 +2711,8 @@
       <c r="D143" s="3">
         <v>19.444444599999997</v>
       </c>
-      <c r="F143">
-        <f t="shared" si="2"/>
-        <v>5.4012346543209864</v>
-      </c>
-    </row>
-    <row r="144" spans="1:6" x14ac:dyDescent="0.35">
+    </row>
+    <row r="144" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A144" s="3" t="s">
         <v>8</v>
       </c>
@@ -3301,12 +2725,8 @@
       <c r="D144" s="3">
         <v>19.444444599999997</v>
       </c>
-      <c r="F144">
-        <f t="shared" si="2"/>
-        <v>5.4012346543209864</v>
-      </c>
-    </row>
-    <row r="145" spans="1:6" x14ac:dyDescent="0.35">
+    </row>
+    <row r="145" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A145" s="3" t="s">
         <v>9</v>
       </c>
@@ -3322,12 +2742,8 @@
       <c r="E145" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="F145">
-        <f t="shared" si="2"/>
-        <v>5.4012346543209864</v>
-      </c>
-    </row>
-    <row r="146" spans="1:6" x14ac:dyDescent="0.35">
+    </row>
+    <row r="146" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A146" s="3" t="s">
         <v>9</v>
       </c>
@@ -3340,12 +2756,8 @@
       <c r="D146" s="3">
         <v>19.444444599999997</v>
       </c>
-      <c r="F146">
-        <f t="shared" si="2"/>
-        <v>5.4012346543209864</v>
-      </c>
-    </row>
-    <row r="147" spans="1:6" x14ac:dyDescent="0.35">
+    </row>
+    <row r="147" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A147" s="3" t="s">
         <v>9</v>
       </c>
@@ -3361,12 +2773,8 @@
       <c r="E147" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="F147">
-        <f t="shared" si="2"/>
-        <v>5.4012346543209864</v>
-      </c>
-    </row>
-    <row r="148" spans="1:6" x14ac:dyDescent="0.35">
+    </row>
+    <row r="148" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A148" s="3" t="s">
         <v>9</v>
       </c>
@@ -3379,12 +2787,8 @@
       <c r="D148" s="3">
         <v>19.444444599999997</v>
       </c>
-      <c r="F148">
-        <f t="shared" si="2"/>
-        <v>5.4012346543209864</v>
-      </c>
-    </row>
-    <row r="149" spans="1:6" x14ac:dyDescent="0.35">
+    </row>
+    <row r="149" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A149" s="3" t="s">
         <v>10</v>
       </c>
@@ -3397,12 +2801,8 @@
       <c r="D149" s="3">
         <v>19.444444599999997</v>
       </c>
-      <c r="F149">
-        <f t="shared" si="2"/>
-        <v>5.4012346543209864</v>
-      </c>
-    </row>
-    <row r="150" spans="1:6" x14ac:dyDescent="0.35">
+    </row>
+    <row r="150" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A150" s="3" t="s">
         <v>10</v>
       </c>
@@ -3415,12 +2815,8 @@
       <c r="D150" s="3">
         <v>19.444444599999997</v>
       </c>
-      <c r="F150">
-        <f t="shared" si="2"/>
-        <v>5.4012346543209864</v>
-      </c>
-    </row>
-    <row r="151" spans="1:6" x14ac:dyDescent="0.35">
+    </row>
+    <row r="151" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A151" s="3" t="s">
         <v>10</v>
       </c>
@@ -3433,12 +2829,8 @@
       <c r="D151" s="3">
         <v>19.444444599999997</v>
       </c>
-      <c r="F151">
-        <f t="shared" si="2"/>
-        <v>5.4012346543209864</v>
-      </c>
-    </row>
-    <row r="152" spans="1:6" x14ac:dyDescent="0.35">
+    </row>
+    <row r="152" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A152" s="3" t="s">
         <v>11</v>
       </c>
@@ -3454,12 +2846,8 @@
       <c r="E152" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="F152">
-        <f t="shared" si="2"/>
-        <v>5.4012346543209864</v>
-      </c>
-    </row>
-    <row r="153" spans="1:6" x14ac:dyDescent="0.35">
+    </row>
+    <row r="153" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A153" s="3" t="s">
         <v>11</v>
       </c>
@@ -3475,12 +2863,8 @@
       <c r="E153" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="F153">
-        <f t="shared" si="2"/>
-        <v>5.4012346543209864</v>
-      </c>
-    </row>
-    <row r="154" spans="1:6" x14ac:dyDescent="0.35">
+    </row>
+    <row r="154" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A154" s="3" t="s">
         <v>11</v>
       </c>
@@ -3496,12 +2880,8 @@
       <c r="E154" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="F154">
-        <f t="shared" si="2"/>
-        <v>5.4012346543209864</v>
-      </c>
-    </row>
-    <row r="155" spans="1:6" x14ac:dyDescent="0.35">
+    </row>
+    <row r="155" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A155" s="3" t="s">
         <v>11</v>
       </c>
@@ -3515,14 +2895,10 @@
         <v>19.444444599999997</v>
       </c>
       <c r="E155" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="F155">
-        <f t="shared" si="2"/>
-        <v>5.4012346543209864</v>
-      </c>
-    </row>
-    <row r="156" spans="1:6" x14ac:dyDescent="0.35">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="156" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A156" s="3" t="s">
         <v>11</v>
       </c>
@@ -3538,12 +2914,8 @@
       <c r="E156" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="F156">
-        <f t="shared" si="2"/>
-        <v>5.4012346543209864</v>
-      </c>
-    </row>
-    <row r="157" spans="1:6" x14ac:dyDescent="0.35">
+    </row>
+    <row r="157" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A157" s="3" t="s">
         <v>11</v>
       </c>
@@ -3559,12 +2931,8 @@
       <c r="E157" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="F157">
-        <f t="shared" si="2"/>
-        <v>5.4012346543209864</v>
-      </c>
-    </row>
-    <row r="158" spans="1:6" x14ac:dyDescent="0.35">
+    </row>
+    <row r="158" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A158" s="3" t="s">
         <v>11</v>
       </c>
@@ -3580,12 +2948,8 @@
       <c r="E158" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="F158">
-        <f t="shared" si="2"/>
-        <v>5.4012346543209864</v>
-      </c>
-    </row>
-    <row r="159" spans="1:6" x14ac:dyDescent="0.35">
+    </row>
+    <row r="159" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A159" s="3" t="s">
         <v>11</v>
       </c>
@@ -3601,12 +2965,8 @@
       <c r="E159" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="F159">
-        <f t="shared" si="2"/>
-        <v>5.4012346543209864</v>
-      </c>
-    </row>
-    <row r="160" spans="1:6" x14ac:dyDescent="0.35">
+    </row>
+    <row r="160" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A160" s="3" t="s">
         <v>11</v>
       </c>
@@ -3622,12 +2982,8 @@
       <c r="E160" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="F160">
-        <f t="shared" si="2"/>
-        <v>5.4012346543209864</v>
-      </c>
-    </row>
-    <row r="161" spans="1:6" x14ac:dyDescent="0.35">
+    </row>
+    <row r="161" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A161" s="3" t="s">
         <v>11</v>
       </c>
@@ -3643,12 +2999,8 @@
       <c r="E161" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="F161">
-        <f t="shared" si="2"/>
-        <v>5.4012346543209864</v>
-      </c>
-    </row>
-    <row r="162" spans="1:6" x14ac:dyDescent="0.35">
+    </row>
+    <row r="162" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A162" s="3" t="s">
         <v>11</v>
       </c>
@@ -3664,12 +3016,8 @@
       <c r="E162" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="F162">
-        <f t="shared" si="2"/>
-        <v>5.4012346543209864</v>
-      </c>
-    </row>
-    <row r="163" spans="1:6" x14ac:dyDescent="0.35">
+    </row>
+    <row r="163" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A163" s="3" t="s">
         <v>11</v>
       </c>
@@ -3685,12 +3033,8 @@
       <c r="E163" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="F163">
-        <f t="shared" si="2"/>
-        <v>5.4012346543209864</v>
-      </c>
-    </row>
-    <row r="164" spans="1:6" x14ac:dyDescent="0.35">
+    </row>
+    <row r="164" spans="1:5" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A164" s="3" t="s">
         <v>11</v>
       </c>
@@ -3706,12 +3050,8 @@
       <c r="E164" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="F164">
-        <f t="shared" si="2"/>
-        <v>5.4012346543209864</v>
-      </c>
-    </row>
-    <row r="165" spans="1:6" x14ac:dyDescent="0.35">
+    </row>
+    <row r="165" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A165" s="3" t="s">
         <v>11</v>
       </c>
@@ -3727,12 +3067,8 @@
       <c r="E165" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="F165">
-        <f t="shared" si="2"/>
-        <v>5.4012346543209864</v>
-      </c>
-    </row>
-    <row r="166" spans="1:6" x14ac:dyDescent="0.35">
+    </row>
+    <row r="166" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A166" s="3" t="s">
         <v>11</v>
       </c>
@@ -3748,12 +3084,8 @@
       <c r="E166" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="F166">
-        <f t="shared" si="2"/>
-        <v>5.4012346543209864</v>
-      </c>
-    </row>
-    <row r="167" spans="1:6" x14ac:dyDescent="0.35">
+    </row>
+    <row r="167" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A167" s="3" t="s">
         <v>11</v>
       </c>
@@ -3769,12 +3101,8 @@
       <c r="E167" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="F167">
-        <f t="shared" si="2"/>
-        <v>5.4012346543209864</v>
-      </c>
-    </row>
-    <row r="168" spans="1:6" x14ac:dyDescent="0.35">
+    </row>
+    <row r="168" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A168" s="3" t="s">
         <v>11</v>
       </c>
@@ -3790,12 +3118,8 @@
       <c r="E168" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="F168">
-        <f t="shared" si="2"/>
-        <v>5.4012346543209864</v>
-      </c>
-    </row>
-    <row r="169" spans="1:6" x14ac:dyDescent="0.35">
+    </row>
+    <row r="169" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A169" s="3" t="s">
         <v>11</v>
       </c>
@@ -3811,12 +3135,8 @@
       <c r="E169" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="F169">
-        <f t="shared" si="2"/>
-        <v>5.4012346543209864</v>
-      </c>
-    </row>
-    <row r="170" spans="1:6" x14ac:dyDescent="0.35">
+    </row>
+    <row r="170" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A170" s="3" t="s">
         <v>11</v>
       </c>
@@ -3832,12 +3152,8 @@
       <c r="E170" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="F170">
-        <f t="shared" si="2"/>
-        <v>5.4012346543209864</v>
-      </c>
-    </row>
-    <row r="171" spans="1:6" x14ac:dyDescent="0.35">
+    </row>
+    <row r="171" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A171" s="3" t="s">
         <v>11</v>
       </c>
@@ -3853,12 +3169,8 @@
       <c r="E171" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="F171">
-        <f t="shared" si="2"/>
-        <v>5.4012346543209864</v>
-      </c>
-    </row>
-    <row r="172" spans="1:6" x14ac:dyDescent="0.35">
+    </row>
+    <row r="172" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A172" s="3" t="s">
         <v>11</v>
       </c>
@@ -3874,12 +3186,8 @@
       <c r="E172" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="F172">
-        <f t="shared" si="2"/>
-        <v>5.4012346543209864</v>
-      </c>
-    </row>
-    <row r="173" spans="1:6" x14ac:dyDescent="0.35">
+    </row>
+    <row r="173" spans="1:5" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A173" s="3" t="s">
         <v>11</v>
       </c>
@@ -3895,14 +3203,10 @@
       <c r="E173" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="F173">
-        <f t="shared" si="2"/>
-        <v>5.4012346543209864</v>
-      </c>
-    </row>
-    <row r="174" spans="1:6" x14ac:dyDescent="0.35">
+    </row>
+    <row r="174" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A174" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B174" s="5">
         <v>151</v>
@@ -3914,14 +3218,10 @@
         <v>27.777777999999998</v>
       </c>
       <c r="E174" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="F174">
-        <f t="shared" si="2"/>
-        <v>7.7160495061728387</v>
-      </c>
-    </row>
-    <row r="175" spans="1:6" x14ac:dyDescent="0.35">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="175" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A175" s="3" t="s">
         <v>12</v>
       </c>
@@ -3937,12 +3237,8 @@
       <c r="E175" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="F175">
-        <f t="shared" si="2"/>
-        <v>4.6296297037037029</v>
-      </c>
-    </row>
-    <row r="176" spans="1:6" x14ac:dyDescent="0.35">
+    </row>
+    <row r="176" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A176" s="3" t="s">
         <v>12</v>
       </c>
@@ -3955,12 +3251,8 @@
       <c r="D176" s="3">
         <v>16.666666799999998</v>
       </c>
-      <c r="F176">
-        <f t="shared" si="2"/>
-        <v>4.6296297037037029</v>
-      </c>
-    </row>
-    <row r="177" spans="1:6" x14ac:dyDescent="0.35">
+    </row>
+    <row r="177" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A177" s="3" t="s">
         <v>12</v>
       </c>
@@ -3973,12 +3265,8 @@
       <c r="D177" s="3">
         <v>16.666666799999998</v>
       </c>
-      <c r="F177">
-        <f t="shared" si="2"/>
-        <v>4.6296297037037029</v>
-      </c>
-    </row>
-    <row r="178" spans="1:6" x14ac:dyDescent="0.35">
+    </row>
+    <row r="178" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A178" s="3" t="s">
         <v>12</v>
       </c>
@@ -3991,102 +3279,98 @@
       <c r="D178" s="3">
         <v>16.666666799999998</v>
       </c>
-      <c r="F178">
-        <f t="shared" si="2"/>
-        <v>4.6296297037037029</v>
-      </c>
-    </row>
-    <row r="194" spans="4:4" x14ac:dyDescent="0.35">
+    </row>
+    <row r="194" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D194" s="3"/>
     </row>
-    <row r="195" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="195" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D195" s="3"/>
     </row>
-    <row r="196" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="196" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D196" s="3"/>
     </row>
-    <row r="197" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="197" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D197" s="3"/>
     </row>
-    <row r="198" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="198" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D198" s="3"/>
     </row>
-    <row r="199" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="199" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D199" s="3"/>
     </row>
-    <row r="200" spans="4:4" x14ac:dyDescent="0.35">
+    <row r="200" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D200" s="3"/>
     </row>
-    <row r="213" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="213" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A213" s="3"/>
       <c r="B213" s="4"/>
       <c r="C213" s="3"/>
       <c r="D213" s="3"/>
       <c r="E213" s="5"/>
     </row>
-    <row r="214" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="214" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A214" s="3"/>
       <c r="B214" s="3"/>
       <c r="C214" s="3"/>
       <c r="D214" s="3"/>
     </row>
-    <row r="215" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="215" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A215" s="3"/>
       <c r="B215" s="3"/>
       <c r="C215" s="3"/>
       <c r="D215" s="3"/>
       <c r="E215" s="5"/>
     </row>
-    <row r="216" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="216" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A216" s="3"/>
       <c r="B216" s="4"/>
       <c r="C216" s="3"/>
       <c r="D216" s="3"/>
     </row>
-    <row r="217" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="217" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A217" s="3"/>
       <c r="B217" s="3"/>
       <c r="C217" s="3"/>
       <c r="D217" s="3"/>
     </row>
-    <row r="218" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="218" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A218" s="3"/>
       <c r="B218" s="4"/>
       <c r="C218" s="3"/>
       <c r="D218" s="3"/>
     </row>
-    <row r="219" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="219" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A219" s="3"/>
       <c r="B219" s="4"/>
       <c r="C219" s="3"/>
       <c r="D219" s="3"/>
     </row>
-    <row r="220" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="220" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A220" s="3"/>
       <c r="B220" s="3"/>
       <c r="C220" s="3"/>
       <c r="D220" s="3"/>
     </row>
-    <row r="221" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="221" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A221" s="3"/>
       <c r="B221" s="3"/>
       <c r="C221" s="3"/>
       <c r="D221" s="3"/>
     </row>
-    <row r="222" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="222" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A222" s="3"/>
       <c r="B222" s="4"/>
       <c r="C222" s="3"/>
       <c r="D222" s="3"/>
     </row>
-    <row r="223" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="223" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A223" s="3"/>
       <c r="B223" s="3"/>
       <c r="C223" s="3"/>
       <c r="D223" s="3"/>
       <c r="E223" s="5"/>
     </row>
-    <row r="224" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="224" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A224" s="3"/>
       <c r="B224" s="3"/>
       <c r="C224" s="3"/>

</xml_diff>